<commit_message>
Added Wrap Text to Report Notes
</commit_message>
<xml_diff>
--- a/Src/SummitReports.Objects/Reports/UWRelationshipCashFlowReport/UW-RCF-Reports.xlsx
+++ b/Src/SummitReports.Objects/Reports/UWRelationshipCashFlowReport/UW-RCF-Reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Summit\SummitReports\Src\SummitReports.Objects\Reports\UWRelationshipCashFlowReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A03724C-1EB1-417B-89AA-4FE527CB5CD8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0A32BA-357B-4CC6-925D-50E05EDC3291}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3398" yWindow="16103" windowWidth="25396" windowHeight="15344" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="25396" windowHeight="15346" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BidPoolData" sheetId="8" state="hidden" r:id="rId1"/>
@@ -753,7 +753,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -818,6 +818,15 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -853,41 +862,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1876,8 +1885,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:R17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1937,11 +1946,11 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="32" t="str">
+      <c r="B3" s="35" t="str">
         <f>RelationshipData!B1</f>
         <v>Donald Trump Mini-Golf</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="36"/>
       <c r="D3" t="s">
         <v>88</v>
       </c>
@@ -1992,11 +2001,11 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="32" t="str">
+      <c r="B5" s="35" t="str">
         <f>RelationshipData!D1</f>
         <v>2nd Penn Bank (2Q19)</v>
       </c>
-      <c r="C5" s="33"/>
+      <c r="C5" s="36"/>
       <c r="F5" t="s">
         <v>102</v>
       </c>
@@ -2078,16 +2087,16 @@
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="32" t="str">
+      <c r="B7" s="35" t="str">
         <f>RelationshipData!U1</f>
         <v>210 Palm Beaqch Lakes Blvd.</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="32" t="str">
+      <c r="C7" s="36"/>
+      <c r="D7" s="35" t="str">
         <f>RelationshipData!V1</f>
         <v>West Palm Beach</v>
       </c>
-      <c r="E7" s="33"/>
+      <c r="E7" s="36"/>
       <c r="F7" s="3" t="str">
         <f>RelationshipData!W1</f>
         <v>FL</v>
@@ -2114,13 +2123,13 @@
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="34" t="str">
+      <c r="B9" s="37" t="str">
         <f>RelationshipData!X1</f>
         <v>36 hole mini golf course and race track</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="35"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="38"/>
       <c r="H9" s="8" t="s">
         <v>106</v>
       </c>
@@ -2166,19 +2175,19 @@
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="34" t="str">
+      <c r="B11" s="37" t="str">
         <f>RelationshipData!O1</f>
         <v>Non-Performing</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="38"/>
       <c r="D11" t="s">
         <v>90</v>
       </c>
-      <c r="E11" s="37" t="str">
+      <c r="E11" s="40" t="str">
         <f>RelationshipData!T1</f>
         <v>18 months chapter 13  then restructure to performing and sell the loan.</v>
       </c>
-      <c r="F11" s="38"/>
+      <c r="F11" s="41"/>
       <c r="M11" s="11" t="s">
         <v>122</v>
       </c>
@@ -2196,13 +2205,13 @@
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="34" t="str">
+      <c r="B12" s="37" t="str">
         <f>RelationshipData!P1</f>
         <v>Performing (Fixed)</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40"/>
+      <c r="C12" s="38"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="43"/>
       <c r="M12" s="13">
         <f>RelationshipData!AW1</f>
         <v>0</v>
@@ -2229,12 +2238,12 @@
         <v>0.12</v>
       </c>
       <c r="C13" s="22"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="30" t="s">
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="H13" s="31"/>
+      <c r="H13" s="34"/>
       <c r="I13" s="4">
         <f>RelationshipData!C2</f>
         <v>35</v>
@@ -2253,34 +2262,34 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="E14" s="41"/>
-      <c r="F14" s="42"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="45"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="52" t="s">
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="53"/>
-      <c r="N16" s="53"/>
-      <c r="O16" s="53"/>
-      <c r="P16" s="53"/>
-      <c r="Q16" s="53"/>
-      <c r="R16" s="54"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="32"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
@@ -2353,8 +2362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5FA1A1-6E42-405D-B2DA-0D63F2AF1F86}">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="T54" sqref="T54"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:R66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2367,384 +2376,384 @@
       <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A2" s="43"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="45"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="48"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="48"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="51"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="48"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="51"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
-      <c r="R5" s="48"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="51"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A6" s="46"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="48"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="51"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A7" s="46"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="48"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="51"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A8" s="46"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="48"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="51"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A9" s="46"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
-      <c r="P9" s="47"/>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="48"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
+      <c r="O9" s="50"/>
+      <c r="P9" s="50"/>
+      <c r="Q9" s="50"/>
+      <c r="R9" s="51"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A10" s="46"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
-      <c r="P10" s="47"/>
-      <c r="Q10" s="47"/>
-      <c r="R10" s="48"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="50"/>
+      <c r="R10" s="51"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A11" s="46"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="47"/>
-      <c r="P11" s="47"/>
-      <c r="Q11" s="47"/>
-      <c r="R11" s="48"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="51"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A12" s="46"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="47"/>
-      <c r="R12" s="48"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="51"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A13" s="46"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="47"/>
-      <c r="P13" s="47"/>
-      <c r="Q13" s="47"/>
-      <c r="R13" s="48"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="50"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="51"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A14" s="46"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47"/>
-      <c r="Q14" s="47"/>
-      <c r="R14" s="48"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="51"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A15" s="46"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
-      <c r="O15" s="47"/>
-      <c r="P15" s="47"/>
-      <c r="Q15" s="47"/>
-      <c r="R15" s="48"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="51"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A16" s="46"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="47"/>
-      <c r="P16" s="47"/>
-      <c r="Q16" s="47"/>
-      <c r="R16" s="48"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="50"/>
+      <c r="P16" s="50"/>
+      <c r="Q16" s="50"/>
+      <c r="R16" s="51"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A17" s="46"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="47"/>
-      <c r="P17" s="47"/>
-      <c r="Q17" s="47"/>
-      <c r="R17" s="48"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="50"/>
+      <c r="P17" s="50"/>
+      <c r="Q17" s="50"/>
+      <c r="R17" s="51"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A18" s="46"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="47"/>
-      <c r="Q18" s="47"/>
-      <c r="R18" s="48"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="50"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="51"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A19" s="46"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="47"/>
-      <c r="Q19" s="47"/>
-      <c r="R19" s="48"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="51"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A20" s="49"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="50"/>
-      <c r="P20" s="50"/>
-      <c r="Q20" s="50"/>
-      <c r="R20" s="51"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="53"/>
+      <c r="R20" s="54"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H21" s="8"/>
@@ -2758,404 +2767,404 @@
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A23" s="43"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="44"/>
-      <c r="O23" s="44"/>
-      <c r="P23" s="44"/>
-      <c r="Q23" s="44"/>
-      <c r="R23" s="45"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="41"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A24" s="46"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="47"/>
-      <c r="P24" s="47"/>
-      <c r="Q24" s="47"/>
-      <c r="R24" s="48"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="56"/>
+      <c r="P24" s="56"/>
+      <c r="Q24" s="56"/>
+      <c r="R24" s="43"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A25" s="46"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="47"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="47"/>
-      <c r="P25" s="47"/>
-      <c r="Q25" s="47"/>
-      <c r="R25" s="48"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="56"/>
+      <c r="P25" s="56"/>
+      <c r="Q25" s="56"/>
+      <c r="R25" s="43"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A26" s="46"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="47"/>
-      <c r="M26" s="47"/>
-      <c r="N26" s="47"/>
-      <c r="O26" s="47"/>
-      <c r="P26" s="47"/>
-      <c r="Q26" s="47"/>
-      <c r="R26" s="48"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="56"/>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="56"/>
+      <c r="R26" s="43"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A27" s="46"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="47"/>
-      <c r="P27" s="47"/>
-      <c r="Q27" s="47"/>
-      <c r="R27" s="48"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="56"/>
+      <c r="P27" s="56"/>
+      <c r="Q27" s="56"/>
+      <c r="R27" s="43"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A28" s="46"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
-      <c r="O28" s="47"/>
-      <c r="P28" s="47"/>
-      <c r="Q28" s="47"/>
-      <c r="R28" s="48"/>
+      <c r="A28" s="42"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="43"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A29" s="46"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="47"/>
-      <c r="P29" s="47"/>
-      <c r="Q29" s="47"/>
-      <c r="R29" s="48"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="43"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A30" s="46"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="47"/>
-      <c r="P30" s="47"/>
-      <c r="Q30" s="47"/>
-      <c r="R30" s="48"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="56"/>
+      <c r="P30" s="56"/>
+      <c r="Q30" s="56"/>
+      <c r="R30" s="43"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A31" s="46"/>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="47"/>
-      <c r="P31" s="47"/>
-      <c r="Q31" s="47"/>
-      <c r="R31" s="48"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="43"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A32" s="46"/>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
-      <c r="P32" s="47"/>
-      <c r="Q32" s="47"/>
-      <c r="R32" s="48"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="56"/>
+      <c r="R32" s="43"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A33" s="46"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
-      <c r="N33" s="47"/>
-      <c r="O33" s="47"/>
-      <c r="P33" s="47"/>
-      <c r="Q33" s="47"/>
-      <c r="R33" s="48"/>
+      <c r="A33" s="42"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="56"/>
+      <c r="O33" s="56"/>
+      <c r="P33" s="56"/>
+      <c r="Q33" s="56"/>
+      <c r="R33" s="43"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A34" s="46"/>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="47"/>
-      <c r="O34" s="47"/>
-      <c r="P34" s="47"/>
-      <c r="Q34" s="47"/>
-      <c r="R34" s="48"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="56"/>
+      <c r="L34" s="56"/>
+      <c r="M34" s="56"/>
+      <c r="N34" s="56"/>
+      <c r="O34" s="56"/>
+      <c r="P34" s="56"/>
+      <c r="Q34" s="56"/>
+      <c r="R34" s="43"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A35" s="46"/>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="47"/>
-      <c r="O35" s="47"/>
-      <c r="P35" s="47"/>
-      <c r="Q35" s="47"/>
-      <c r="R35" s="48"/>
+      <c r="A35" s="42"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="56"/>
+      <c r="O35" s="56"/>
+      <c r="P35" s="56"/>
+      <c r="Q35" s="56"/>
+      <c r="R35" s="43"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A36" s="46"/>
-      <c r="B36" s="47"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
-      <c r="N36" s="47"/>
-      <c r="O36" s="47"/>
-      <c r="P36" s="47"/>
-      <c r="Q36" s="47"/>
-      <c r="R36" s="48"/>
+      <c r="A36" s="42"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="56"/>
+      <c r="K36" s="56"/>
+      <c r="L36" s="56"/>
+      <c r="M36" s="56"/>
+      <c r="N36" s="56"/>
+      <c r="O36" s="56"/>
+      <c r="P36" s="56"/>
+      <c r="Q36" s="56"/>
+      <c r="R36" s="43"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A37" s="46"/>
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="47"/>
-      <c r="L37" s="47"/>
-      <c r="M37" s="47"/>
-      <c r="N37" s="47"/>
-      <c r="O37" s="47"/>
-      <c r="P37" s="47"/>
-      <c r="Q37" s="47"/>
-      <c r="R37" s="48"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="56"/>
+      <c r="M37" s="56"/>
+      <c r="N37" s="56"/>
+      <c r="O37" s="56"/>
+      <c r="P37" s="56"/>
+      <c r="Q37" s="56"/>
+      <c r="R37" s="43"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A38" s="46"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="47"/>
-      <c r="K38" s="47"/>
-      <c r="L38" s="47"/>
-      <c r="M38" s="47"/>
-      <c r="N38" s="47"/>
-      <c r="O38" s="47"/>
-      <c r="P38" s="47"/>
-      <c r="Q38" s="47"/>
-      <c r="R38" s="48"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="56"/>
+      <c r="J38" s="56"/>
+      <c r="K38" s="56"/>
+      <c r="L38" s="56"/>
+      <c r="M38" s="56"/>
+      <c r="N38" s="56"/>
+      <c r="O38" s="56"/>
+      <c r="P38" s="56"/>
+      <c r="Q38" s="56"/>
+      <c r="R38" s="43"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A39" s="46"/>
-      <c r="B39" s="47"/>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="47"/>
-      <c r="J39" s="47"/>
-      <c r="K39" s="47"/>
-      <c r="L39" s="47"/>
-      <c r="M39" s="47"/>
-      <c r="N39" s="47"/>
-      <c r="O39" s="47"/>
-      <c r="P39" s="47"/>
-      <c r="Q39" s="47"/>
-      <c r="R39" s="48"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="56"/>
+      <c r="J39" s="56"/>
+      <c r="K39" s="56"/>
+      <c r="L39" s="56"/>
+      <c r="M39" s="56"/>
+      <c r="N39" s="56"/>
+      <c r="O39" s="56"/>
+      <c r="P39" s="56"/>
+      <c r="Q39" s="56"/>
+      <c r="R39" s="43"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A40" s="46"/>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="47"/>
-      <c r="L40" s="47"/>
-      <c r="M40" s="47"/>
-      <c r="N40" s="47"/>
-      <c r="O40" s="47"/>
-      <c r="P40" s="47"/>
-      <c r="Q40" s="47"/>
-      <c r="R40" s="48"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="56"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="56"/>
+      <c r="J40" s="56"/>
+      <c r="K40" s="56"/>
+      <c r="L40" s="56"/>
+      <c r="M40" s="56"/>
+      <c r="N40" s="56"/>
+      <c r="O40" s="56"/>
+      <c r="P40" s="56"/>
+      <c r="Q40" s="56"/>
+      <c r="R40" s="43"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A41" s="46"/>
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="47"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="47"/>
-      <c r="M41" s="47"/>
-      <c r="N41" s="47"/>
-      <c r="O41" s="47"/>
-      <c r="P41" s="47"/>
-      <c r="Q41" s="47"/>
-      <c r="R41" s="48"/>
+      <c r="A41" s="42"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="56"/>
+      <c r="G41" s="56"/>
+      <c r="H41" s="56"/>
+      <c r="I41" s="56"/>
+      <c r="J41" s="56"/>
+      <c r="K41" s="56"/>
+      <c r="L41" s="56"/>
+      <c r="M41" s="56"/>
+      <c r="N41" s="56"/>
+      <c r="O41" s="56"/>
+      <c r="P41" s="56"/>
+      <c r="Q41" s="56"/>
+      <c r="R41" s="43"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A42" s="49"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="50"/>
-      <c r="E42" s="50"/>
-      <c r="F42" s="50"/>
-      <c r="G42" s="50"/>
-      <c r="H42" s="50"/>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
-      <c r="K42" s="50"/>
-      <c r="L42" s="50"/>
-      <c r="M42" s="50"/>
-      <c r="N42" s="50"/>
-      <c r="O42" s="50"/>
-      <c r="P42" s="50"/>
-      <c r="Q42" s="50"/>
-      <c r="R42" s="51"/>
+      <c r="A42" s="44"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="57"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="57"/>
+      <c r="K42" s="57"/>
+      <c r="L42" s="57"/>
+      <c r="M42" s="57"/>
+      <c r="N42" s="57"/>
+      <c r="O42" s="57"/>
+      <c r="P42" s="57"/>
+      <c r="Q42" s="57"/>
+      <c r="R42" s="45"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A43" s="24"/>
@@ -3200,204 +3209,204 @@
       <c r="R44" s="24"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A45" s="43"/>
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="44"/>
-      <c r="L45" s="44"/>
-      <c r="M45" s="44"/>
-      <c r="N45" s="44"/>
-      <c r="O45" s="44"/>
-      <c r="P45" s="44"/>
-      <c r="Q45" s="44"/>
-      <c r="R45" s="45"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="55"/>
+      <c r="L45" s="55"/>
+      <c r="M45" s="55"/>
+      <c r="N45" s="55"/>
+      <c r="O45" s="55"/>
+      <c r="P45" s="55"/>
+      <c r="Q45" s="55"/>
+      <c r="R45" s="41"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A46" s="46"/>
-      <c r="B46" s="47"/>
-      <c r="C46" s="47"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="47"/>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
-      <c r="K46" s="47"/>
-      <c r="L46" s="47"/>
-      <c r="M46" s="47"/>
-      <c r="N46" s="47"/>
-      <c r="O46" s="47"/>
-      <c r="P46" s="47"/>
-      <c r="Q46" s="47"/>
-      <c r="R46" s="48"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="56"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="56"/>
+      <c r="L46" s="56"/>
+      <c r="M46" s="56"/>
+      <c r="N46" s="56"/>
+      <c r="O46" s="56"/>
+      <c r="P46" s="56"/>
+      <c r="Q46" s="56"/>
+      <c r="R46" s="43"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A47" s="46"/>
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="47"/>
-      <c r="I47" s="47"/>
-      <c r="J47" s="47"/>
-      <c r="K47" s="47"/>
-      <c r="L47" s="47"/>
-      <c r="M47" s="47"/>
-      <c r="N47" s="47"/>
-      <c r="O47" s="47"/>
-      <c r="P47" s="47"/>
-      <c r="Q47" s="47"/>
-      <c r="R47" s="48"/>
+      <c r="A47" s="42"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="56"/>
+      <c r="G47" s="56"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="56"/>
+      <c r="L47" s="56"/>
+      <c r="M47" s="56"/>
+      <c r="N47" s="56"/>
+      <c r="O47" s="56"/>
+      <c r="P47" s="56"/>
+      <c r="Q47" s="56"/>
+      <c r="R47" s="43"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A48" s="46"/>
-      <c r="B48" s="47"/>
-      <c r="C48" s="47"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="47"/>
-      <c r="I48" s="47"/>
-      <c r="J48" s="47"/>
-      <c r="K48" s="47"/>
-      <c r="L48" s="47"/>
-      <c r="M48" s="47"/>
-      <c r="N48" s="47"/>
-      <c r="O48" s="47"/>
-      <c r="P48" s="47"/>
-      <c r="Q48" s="47"/>
-      <c r="R48" s="48"/>
+      <c r="A48" s="42"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="56"/>
+      <c r="I48" s="56"/>
+      <c r="J48" s="56"/>
+      <c r="K48" s="56"/>
+      <c r="L48" s="56"/>
+      <c r="M48" s="56"/>
+      <c r="N48" s="56"/>
+      <c r="O48" s="56"/>
+      <c r="P48" s="56"/>
+      <c r="Q48" s="56"/>
+      <c r="R48" s="43"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A49" s="46"/>
-      <c r="B49" s="47"/>
-      <c r="C49" s="47"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="47"/>
-      <c r="F49" s="47"/>
-      <c r="G49" s="47"/>
-      <c r="H49" s="47"/>
-      <c r="I49" s="47"/>
-      <c r="J49" s="47"/>
-      <c r="K49" s="47"/>
-      <c r="L49" s="47"/>
-      <c r="M49" s="47"/>
-      <c r="N49" s="47"/>
-      <c r="O49" s="47"/>
-      <c r="P49" s="47"/>
-      <c r="Q49" s="47"/>
-      <c r="R49" s="48"/>
+      <c r="A49" s="42"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="56"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="56"/>
+      <c r="I49" s="56"/>
+      <c r="J49" s="56"/>
+      <c r="K49" s="56"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="56"/>
+      <c r="N49" s="56"/>
+      <c r="O49" s="56"/>
+      <c r="P49" s="56"/>
+      <c r="Q49" s="56"/>
+      <c r="R49" s="43"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A50" s="46"/>
-      <c r="B50" s="47"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
-      <c r="H50" s="47"/>
-      <c r="I50" s="47"/>
-      <c r="J50" s="47"/>
-      <c r="K50" s="47"/>
-      <c r="L50" s="47"/>
-      <c r="M50" s="47"/>
-      <c r="N50" s="47"/>
-      <c r="O50" s="47"/>
-      <c r="P50" s="47"/>
-      <c r="Q50" s="47"/>
-      <c r="R50" s="48"/>
+      <c r="A50" s="42"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="56"/>
+      <c r="H50" s="56"/>
+      <c r="I50" s="56"/>
+      <c r="J50" s="56"/>
+      <c r="K50" s="56"/>
+      <c r="L50" s="56"/>
+      <c r="M50" s="56"/>
+      <c r="N50" s="56"/>
+      <c r="O50" s="56"/>
+      <c r="P50" s="56"/>
+      <c r="Q50" s="56"/>
+      <c r="R50" s="43"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A51" s="46"/>
-      <c r="B51" s="47"/>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="47"/>
-      <c r="K51" s="47"/>
-      <c r="L51" s="47"/>
-      <c r="M51" s="47"/>
-      <c r="N51" s="47"/>
-      <c r="O51" s="47"/>
-      <c r="P51" s="47"/>
-      <c r="Q51" s="47"/>
-      <c r="R51" s="48"/>
+      <c r="A51" s="42"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="56"/>
+      <c r="J51" s="56"/>
+      <c r="K51" s="56"/>
+      <c r="L51" s="56"/>
+      <c r="M51" s="56"/>
+      <c r="N51" s="56"/>
+      <c r="O51" s="56"/>
+      <c r="P51" s="56"/>
+      <c r="Q51" s="56"/>
+      <c r="R51" s="43"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A52" s="46"/>
-      <c r="B52" s="47"/>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
-      <c r="I52" s="47"/>
-      <c r="J52" s="47"/>
-      <c r="K52" s="47"/>
-      <c r="L52" s="47"/>
-      <c r="M52" s="47"/>
-      <c r="N52" s="47"/>
-      <c r="O52" s="47"/>
-      <c r="P52" s="47"/>
-      <c r="Q52" s="47"/>
-      <c r="R52" s="48"/>
+      <c r="A52" s="42"/>
+      <c r="B52" s="56"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="56"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="56"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="56"/>
+      <c r="I52" s="56"/>
+      <c r="J52" s="56"/>
+      <c r="K52" s="56"/>
+      <c r="L52" s="56"/>
+      <c r="M52" s="56"/>
+      <c r="N52" s="56"/>
+      <c r="O52" s="56"/>
+      <c r="P52" s="56"/>
+      <c r="Q52" s="56"/>
+      <c r="R52" s="43"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A53" s="46"/>
-      <c r="B53" s="47"/>
-      <c r="C53" s="47"/>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="47"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="47"/>
-      <c r="I53" s="47"/>
-      <c r="J53" s="47"/>
-      <c r="K53" s="47"/>
-      <c r="L53" s="47"/>
-      <c r="M53" s="47"/>
-      <c r="N53" s="47"/>
-      <c r="O53" s="47"/>
-      <c r="P53" s="47"/>
-      <c r="Q53" s="47"/>
-      <c r="R53" s="48"/>
+      <c r="A53" s="42"/>
+      <c r="B53" s="56"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="56"/>
+      <c r="H53" s="56"/>
+      <c r="I53" s="56"/>
+      <c r="J53" s="56"/>
+      <c r="K53" s="56"/>
+      <c r="L53" s="56"/>
+      <c r="M53" s="56"/>
+      <c r="N53" s="56"/>
+      <c r="O53" s="56"/>
+      <c r="P53" s="56"/>
+      <c r="Q53" s="56"/>
+      <c r="R53" s="43"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A54" s="49"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="50"/>
-      <c r="D54" s="50"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="50"/>
-      <c r="G54" s="50"/>
-      <c r="H54" s="50"/>
-      <c r="I54" s="50"/>
-      <c r="J54" s="50"/>
-      <c r="K54" s="50"/>
-      <c r="L54" s="50"/>
-      <c r="M54" s="50"/>
-      <c r="N54" s="50"/>
-      <c r="O54" s="50"/>
-      <c r="P54" s="50"/>
-      <c r="Q54" s="50"/>
-      <c r="R54" s="51"/>
+      <c r="A54" s="44"/>
+      <c r="B54" s="57"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="57"/>
+      <c r="E54" s="57"/>
+      <c r="F54" s="57"/>
+      <c r="G54" s="57"/>
+      <c r="H54" s="57"/>
+      <c r="I54" s="57"/>
+      <c r="J54" s="57"/>
+      <c r="K54" s="57"/>
+      <c r="L54" s="57"/>
+      <c r="M54" s="57"/>
+      <c r="N54" s="57"/>
+      <c r="O54" s="57"/>
+      <c r="P54" s="57"/>
+      <c r="Q54" s="57"/>
+      <c r="R54" s="45"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H55" s="8"/>
@@ -3426,204 +3435,204 @@
       <c r="R56" s="24"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A57" s="43"/>
-      <c r="B57" s="44"/>
-      <c r="C57" s="44"/>
-      <c r="D57" s="44"/>
-      <c r="E57" s="44"/>
-      <c r="F57" s="44"/>
-      <c r="G57" s="44"/>
-      <c r="H57" s="44"/>
-      <c r="I57" s="44"/>
-      <c r="J57" s="44"/>
-      <c r="K57" s="44"/>
-      <c r="L57" s="44"/>
-      <c r="M57" s="44"/>
-      <c r="N57" s="44"/>
-      <c r="O57" s="44"/>
-      <c r="P57" s="44"/>
-      <c r="Q57" s="44"/>
-      <c r="R57" s="45"/>
+      <c r="A57" s="40"/>
+      <c r="B57" s="55"/>
+      <c r="C57" s="55"/>
+      <c r="D57" s="55"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="55"/>
+      <c r="G57" s="55"/>
+      <c r="H57" s="55"/>
+      <c r="I57" s="55"/>
+      <c r="J57" s="55"/>
+      <c r="K57" s="55"/>
+      <c r="L57" s="55"/>
+      <c r="M57" s="55"/>
+      <c r="N57" s="55"/>
+      <c r="O57" s="55"/>
+      <c r="P57" s="55"/>
+      <c r="Q57" s="55"/>
+      <c r="R57" s="41"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A58" s="46"/>
-      <c r="B58" s="47"/>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
-      <c r="H58" s="47"/>
-      <c r="I58" s="47"/>
-      <c r="J58" s="47"/>
-      <c r="K58" s="47"/>
-      <c r="L58" s="47"/>
-      <c r="M58" s="47"/>
-      <c r="N58" s="47"/>
-      <c r="O58" s="47"/>
-      <c r="P58" s="47"/>
-      <c r="Q58" s="47"/>
-      <c r="R58" s="48"/>
+      <c r="A58" s="42"/>
+      <c r="B58" s="56"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="56"/>
+      <c r="F58" s="56"/>
+      <c r="G58" s="56"/>
+      <c r="H58" s="56"/>
+      <c r="I58" s="56"/>
+      <c r="J58" s="56"/>
+      <c r="K58" s="56"/>
+      <c r="L58" s="56"/>
+      <c r="M58" s="56"/>
+      <c r="N58" s="56"/>
+      <c r="O58" s="56"/>
+      <c r="P58" s="56"/>
+      <c r="Q58" s="56"/>
+      <c r="R58" s="43"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A59" s="46"/>
-      <c r="B59" s="47"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="47"/>
-      <c r="H59" s="47"/>
-      <c r="I59" s="47"/>
-      <c r="J59" s="47"/>
-      <c r="K59" s="47"/>
-      <c r="L59" s="47"/>
-      <c r="M59" s="47"/>
-      <c r="N59" s="47"/>
-      <c r="O59" s="47"/>
-      <c r="P59" s="47"/>
-      <c r="Q59" s="47"/>
-      <c r="R59" s="48"/>
+      <c r="A59" s="42"/>
+      <c r="B59" s="56"/>
+      <c r="C59" s="56"/>
+      <c r="D59" s="56"/>
+      <c r="E59" s="56"/>
+      <c r="F59" s="56"/>
+      <c r="G59" s="56"/>
+      <c r="H59" s="56"/>
+      <c r="I59" s="56"/>
+      <c r="J59" s="56"/>
+      <c r="K59" s="56"/>
+      <c r="L59" s="56"/>
+      <c r="M59" s="56"/>
+      <c r="N59" s="56"/>
+      <c r="O59" s="56"/>
+      <c r="P59" s="56"/>
+      <c r="Q59" s="56"/>
+      <c r="R59" s="43"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A60" s="46"/>
-      <c r="B60" s="47"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="47"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="47"/>
-      <c r="H60" s="47"/>
-      <c r="I60" s="47"/>
-      <c r="J60" s="47"/>
-      <c r="K60" s="47"/>
-      <c r="L60" s="47"/>
-      <c r="M60" s="47"/>
-      <c r="N60" s="47"/>
-      <c r="O60" s="47"/>
-      <c r="P60" s="47"/>
-      <c r="Q60" s="47"/>
-      <c r="R60" s="48"/>
+      <c r="A60" s="42"/>
+      <c r="B60" s="56"/>
+      <c r="C60" s="56"/>
+      <c r="D60" s="56"/>
+      <c r="E60" s="56"/>
+      <c r="F60" s="56"/>
+      <c r="G60" s="56"/>
+      <c r="H60" s="56"/>
+      <c r="I60" s="56"/>
+      <c r="J60" s="56"/>
+      <c r="K60" s="56"/>
+      <c r="L60" s="56"/>
+      <c r="M60" s="56"/>
+      <c r="N60" s="56"/>
+      <c r="O60" s="56"/>
+      <c r="P60" s="56"/>
+      <c r="Q60" s="56"/>
+      <c r="R60" s="43"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A61" s="46"/>
-      <c r="B61" s="47"/>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="47"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="47"/>
-      <c r="H61" s="47"/>
-      <c r="I61" s="47"/>
-      <c r="J61" s="47"/>
-      <c r="K61" s="47"/>
-      <c r="L61" s="47"/>
-      <c r="M61" s="47"/>
-      <c r="N61" s="47"/>
-      <c r="O61" s="47"/>
-      <c r="P61" s="47"/>
-      <c r="Q61" s="47"/>
-      <c r="R61" s="48"/>
+      <c r="A61" s="42"/>
+      <c r="B61" s="56"/>
+      <c r="C61" s="56"/>
+      <c r="D61" s="56"/>
+      <c r="E61" s="56"/>
+      <c r="F61" s="56"/>
+      <c r="G61" s="56"/>
+      <c r="H61" s="56"/>
+      <c r="I61" s="56"/>
+      <c r="J61" s="56"/>
+      <c r="K61" s="56"/>
+      <c r="L61" s="56"/>
+      <c r="M61" s="56"/>
+      <c r="N61" s="56"/>
+      <c r="O61" s="56"/>
+      <c r="P61" s="56"/>
+      <c r="Q61" s="56"/>
+      <c r="R61" s="43"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A62" s="46"/>
-      <c r="B62" s="47"/>
-      <c r="C62" s="47"/>
-      <c r="D62" s="47"/>
-      <c r="E62" s="47"/>
-      <c r="F62" s="47"/>
-      <c r="G62" s="47"/>
-      <c r="H62" s="47"/>
-      <c r="I62" s="47"/>
-      <c r="J62" s="47"/>
-      <c r="K62" s="47"/>
-      <c r="L62" s="47"/>
-      <c r="M62" s="47"/>
-      <c r="N62" s="47"/>
-      <c r="O62" s="47"/>
-      <c r="P62" s="47"/>
-      <c r="Q62" s="47"/>
-      <c r="R62" s="48"/>
+      <c r="A62" s="42"/>
+      <c r="B62" s="56"/>
+      <c r="C62" s="56"/>
+      <c r="D62" s="56"/>
+      <c r="E62" s="56"/>
+      <c r="F62" s="56"/>
+      <c r="G62" s="56"/>
+      <c r="H62" s="56"/>
+      <c r="I62" s="56"/>
+      <c r="J62" s="56"/>
+      <c r="K62" s="56"/>
+      <c r="L62" s="56"/>
+      <c r="M62" s="56"/>
+      <c r="N62" s="56"/>
+      <c r="O62" s="56"/>
+      <c r="P62" s="56"/>
+      <c r="Q62" s="56"/>
+      <c r="R62" s="43"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A63" s="46"/>
-      <c r="B63" s="47"/>
-      <c r="C63" s="47"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="47"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="47"/>
-      <c r="H63" s="47"/>
-      <c r="I63" s="47"/>
-      <c r="J63" s="47"/>
-      <c r="K63" s="47"/>
-      <c r="L63" s="47"/>
-      <c r="M63" s="47"/>
-      <c r="N63" s="47"/>
-      <c r="O63" s="47"/>
-      <c r="P63" s="47"/>
-      <c r="Q63" s="47"/>
-      <c r="R63" s="48"/>
+      <c r="A63" s="42"/>
+      <c r="B63" s="56"/>
+      <c r="C63" s="56"/>
+      <c r="D63" s="56"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="56"/>
+      <c r="G63" s="56"/>
+      <c r="H63" s="56"/>
+      <c r="I63" s="56"/>
+      <c r="J63" s="56"/>
+      <c r="K63" s="56"/>
+      <c r="L63" s="56"/>
+      <c r="M63" s="56"/>
+      <c r="N63" s="56"/>
+      <c r="O63" s="56"/>
+      <c r="P63" s="56"/>
+      <c r="Q63" s="56"/>
+      <c r="R63" s="43"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A64" s="46"/>
-      <c r="B64" s="47"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="47"/>
-      <c r="H64" s="47"/>
-      <c r="I64" s="47"/>
-      <c r="J64" s="47"/>
-      <c r="K64" s="47"/>
-      <c r="L64" s="47"/>
-      <c r="M64" s="47"/>
-      <c r="N64" s="47"/>
-      <c r="O64" s="47"/>
-      <c r="P64" s="47"/>
-      <c r="Q64" s="47"/>
-      <c r="R64" s="48"/>
+      <c r="A64" s="42"/>
+      <c r="B64" s="56"/>
+      <c r="C64" s="56"/>
+      <c r="D64" s="56"/>
+      <c r="E64" s="56"/>
+      <c r="F64" s="56"/>
+      <c r="G64" s="56"/>
+      <c r="H64" s="56"/>
+      <c r="I64" s="56"/>
+      <c r="J64" s="56"/>
+      <c r="K64" s="56"/>
+      <c r="L64" s="56"/>
+      <c r="M64" s="56"/>
+      <c r="N64" s="56"/>
+      <c r="O64" s="56"/>
+      <c r="P64" s="56"/>
+      <c r="Q64" s="56"/>
+      <c r="R64" s="43"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A65" s="46"/>
-      <c r="B65" s="47"/>
-      <c r="C65" s="47"/>
-      <c r="D65" s="47"/>
-      <c r="E65" s="47"/>
-      <c r="F65" s="47"/>
-      <c r="G65" s="47"/>
-      <c r="H65" s="47"/>
-      <c r="I65" s="47"/>
-      <c r="J65" s="47"/>
-      <c r="K65" s="47"/>
-      <c r="L65" s="47"/>
-      <c r="M65" s="47"/>
-      <c r="N65" s="47"/>
-      <c r="O65" s="47"/>
-      <c r="P65" s="47"/>
-      <c r="Q65" s="47"/>
-      <c r="R65" s="48"/>
+      <c r="A65" s="42"/>
+      <c r="B65" s="56"/>
+      <c r="C65" s="56"/>
+      <c r="D65" s="56"/>
+      <c r="E65" s="56"/>
+      <c r="F65" s="56"/>
+      <c r="G65" s="56"/>
+      <c r="H65" s="56"/>
+      <c r="I65" s="56"/>
+      <c r="J65" s="56"/>
+      <c r="K65" s="56"/>
+      <c r="L65" s="56"/>
+      <c r="M65" s="56"/>
+      <c r="N65" s="56"/>
+      <c r="O65" s="56"/>
+      <c r="P65" s="56"/>
+      <c r="Q65" s="56"/>
+      <c r="R65" s="43"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A66" s="49"/>
-      <c r="B66" s="50"/>
-      <c r="C66" s="50"/>
-      <c r="D66" s="50"/>
-      <c r="E66" s="50"/>
-      <c r="F66" s="50"/>
-      <c r="G66" s="50"/>
-      <c r="H66" s="50"/>
-      <c r="I66" s="50"/>
-      <c r="J66" s="50"/>
-      <c r="K66" s="50"/>
-      <c r="L66" s="50"/>
-      <c r="M66" s="50"/>
-      <c r="N66" s="50"/>
-      <c r="O66" s="50"/>
-      <c r="P66" s="50"/>
-      <c r="Q66" s="50"/>
-      <c r="R66" s="51"/>
+      <c r="A66" s="44"/>
+      <c r="B66" s="57"/>
+      <c r="C66" s="57"/>
+      <c r="D66" s="57"/>
+      <c r="E66" s="57"/>
+      <c r="F66" s="57"/>
+      <c r="G66" s="57"/>
+      <c r="H66" s="57"/>
+      <c r="I66" s="57"/>
+      <c r="J66" s="57"/>
+      <c r="K66" s="57"/>
+      <c r="L66" s="57"/>
+      <c r="M66" s="57"/>
+      <c r="N66" s="57"/>
+      <c r="O66" s="57"/>
+      <c r="P66" s="57"/>
+      <c r="Q66" s="57"/>
+      <c r="R66" s="45"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H67" s="8"/>
@@ -3649,5 +3658,6 @@
     <mergeCell ref="A57:R66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a column between Income and Expense
</commit_message>
<xml_diff>
--- a/Src/SummitReports.Objects/Reports/UWRelationshipCashFlowReport/UW-RCF-Reports.xlsx
+++ b/Src/SummitReports.Objects/Reports/UWRelationshipCashFlowReport/UW-RCF-Reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Summit\SummitReports\Src\SummitReports.Objects\Reports\UWRelationshipCashFlowReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0A32BA-357B-4CC6-925D-50E05EDC3291}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C46BE03-0899-4860-B463-6B92120336B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="25396" windowHeight="15346" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BidPoolData" sheetId="8" state="hidden" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="167">
   <si>
     <t>011 : BB&amp;T 2Q18</t>
   </si>
@@ -753,7 +753,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -818,6 +818,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1188,12 +1191,12 @@
       <selection activeCell="B20" sqref="B20:I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.1328125" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>147</v>
       </c>
@@ -1201,77 +1204,77 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1290,20 +1293,20 @@
       <selection activeCell="B20" sqref="B20:I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="18" max="18" width="15.1328125" customWidth="1"/>
-    <col min="19" max="19" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.265625" customWidth="1"/>
-    <col min="22" max="22" width="14.86328125" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.28515625" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" customWidth="1"/>
     <col min="23" max="23" width="16" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="21" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>106</v>
       </c>
@@ -1455,7 +1458,7 @@
       <c r="BF1" s="1"/>
       <c r="BL1" s="1"/>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>106</v>
       </c>
@@ -1472,7 +1475,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1672,7 +1675,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>17</v>
       </c>
@@ -1872,7 +1875,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
   </sheetData>
@@ -1883,24 +1886,24 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8FA40D-F3F7-4105-8B77-A0262887423C}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:R17"/>
+  <dimension ref="A2:S17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.265625" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="7" width="14.265625" customWidth="1"/>
-    <col min="8" max="8" width="14.265625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="14.265625" style="5" customWidth="1"/>
-    <col min="10" max="18" width="14.265625" customWidth="1"/>
+    <col min="5" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="5" customWidth="1"/>
+    <col min="10" max="18" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1942,15 +1945,15 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="35" t="str">
+      <c r="B3" s="36" t="str">
         <f>RelationshipData!B1</f>
         <v>Donald Trump Mini-Golf</v>
       </c>
-      <c r="C3" s="36"/>
+      <c r="C3" s="37"/>
       <c r="D3" t="s">
         <v>88</v>
       </c>
@@ -1993,19 +1996,19 @@
         <v>0.965034965034965</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="35" t="str">
+      <c r="B5" s="36" t="str">
         <f>RelationshipData!D1</f>
         <v>2nd Penn Bank (2Q19)</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="37"/>
       <c r="F5" t="s">
         <v>102</v>
       </c>
@@ -2035,7 +2038,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2083,27 +2086,27 @@
         <v>0.95833333333333337</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="35" t="str">
+      <c r="B7" s="36" t="str">
         <f>RelationshipData!U1</f>
         <v>210 Palm Beaqch Lakes Blvd.</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="35" t="str">
+      <c r="C7" s="37"/>
+      <c r="D7" s="36" t="str">
         <f>RelationshipData!V1</f>
         <v>West Palm Beach</v>
       </c>
-      <c r="E7" s="36"/>
+      <c r="E7" s="37"/>
       <c r="F7" s="3" t="str">
         <f>RelationshipData!W1</f>
         <v>FL</v>
       </c>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H8"/>
       <c r="I8" s="18"/>
       <c r="M8" s="11" t="s">
@@ -2119,17 +2122,17 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="37" t="str">
+      <c r="B9" s="38" t="str">
         <f>RelationshipData!X1</f>
         <v>36 hole mini golf course and race track</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="38"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="39"/>
       <c r="H9" s="8" t="s">
         <v>106</v>
       </c>
@@ -2154,7 +2157,7 @@
         <v>2.8985507246376812E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2171,23 +2174,23 @@
         <v>Bankruptcy</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="37" t="str">
+      <c r="B11" s="38" t="str">
         <f>RelationshipData!O1</f>
         <v>Non-Performing</v>
       </c>
-      <c r="C11" s="38"/>
+      <c r="C11" s="39"/>
       <c r="D11" t="s">
         <v>90</v>
       </c>
-      <c r="E11" s="40" t="str">
+      <c r="E11" s="41" t="str">
         <f>RelationshipData!T1</f>
         <v>18 months chapter 13  then restructure to performing and sell the loan.</v>
       </c>
-      <c r="F11" s="41"/>
+      <c r="F11" s="42"/>
       <c r="M11" s="11" t="s">
         <v>122</v>
       </c>
@@ -2201,17 +2204,17 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="37" t="str">
+      <c r="B12" s="38" t="str">
         <f>RelationshipData!P1</f>
         <v>Performing (Fixed)</v>
       </c>
-      <c r="C12" s="38"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="43"/>
+      <c r="C12" s="39"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="44"/>
       <c r="M12" s="13">
         <f>RelationshipData!AW1</f>
         <v>0</v>
@@ -2229,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2238,12 +2241,12 @@
         <v>0.12</v>
       </c>
       <c r="C13" s="22"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="33" t="s">
+      <c r="E13" s="43"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="H13" s="34"/>
+      <c r="H13" s="35"/>
       <c r="I13" s="4">
         <f>RelationshipData!C2</f>
         <v>35</v>
@@ -2261,37 +2264,37 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="E14" s="44"/>
-      <c r="F14" s="45"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E14" s="45"/>
+      <c r="F14" s="46"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="C16" s="30" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C16" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="30" t="s">
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
+      <c r="J16" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="31"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
       <c r="R16" s="32"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="S16" s="33"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>126</v>
       </c>
@@ -2308,41 +2311,44 @@
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
-      <c r="I17" s="26" t="s">
+      <c r="I17" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="J17" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="J17" s="16" t="s">
+      <c r="K17" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="K17" s="16" t="s">
+      <c r="L17" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="L17" s="16" t="s">
+      <c r="M17" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="M17" s="16" t="s">
+      <c r="N17" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="N17" s="16" t="s">
+      <c r="O17" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="O17" s="16" t="s">
+      <c r="P17" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="P17" s="16" t="s">
+      <c r="Q17" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="Q17" s="16" t="s">
+      <c r="R17" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>138</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="C16:H16"/>
-    <mergeCell ref="I16:R16"/>
+    <mergeCell ref="J16:S16"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B5:C5"/>
@@ -2362,811 +2368,811 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5FA1A1-6E42-405D-B2DA-0D63F2AF1F86}">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A57" sqref="A57:R66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
         <v>142</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="48"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="51"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A4" s="49"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="50"/>
-      <c r="R4" s="51"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="51"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A6" s="49"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="50"/>
-      <c r="R6" s="51"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A7" s="49"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="51"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A8" s="49"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="51"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A9" s="49"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="50"/>
-      <c r="O9" s="50"/>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="51"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A10" s="49"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="50"/>
-      <c r="P10" s="50"/>
-      <c r="Q10" s="50"/>
-      <c r="R10" s="51"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A11" s="49"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="50"/>
-      <c r="P11" s="50"/>
-      <c r="Q11" s="50"/>
-      <c r="R11" s="51"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A12" s="49"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50"/>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="51"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="50"/>
-      <c r="P13" s="50"/>
-      <c r="Q13" s="50"/>
-      <c r="R13" s="51"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A14" s="49"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="50"/>
-      <c r="P14" s="50"/>
-      <c r="Q14" s="50"/>
-      <c r="R14" s="51"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A15" s="49"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="50"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="51"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A16" s="49"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="50"/>
-      <c r="P16" s="50"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="51"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A17" s="49"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="50"/>
-      <c r="O17" s="50"/>
-      <c r="P17" s="50"/>
-      <c r="Q17" s="50"/>
-      <c r="R17" s="51"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A18" s="49"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="50"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="50"/>
-      <c r="R18" s="51"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A19" s="49"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="50"/>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="50"/>
-      <c r="R19" s="51"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A20" s="52"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
-      <c r="N20" s="53"/>
-      <c r="O20" s="53"/>
-      <c r="P20" s="53"/>
-      <c r="Q20" s="53"/>
-      <c r="R20" s="54"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="49"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="52"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="52"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="50"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="52"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="50"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="51"/>
+      <c r="R6" s="52"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="50"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="52"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="50"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="52"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="50"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="52"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="50"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="52"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="50"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="52"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="50"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="52"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="50"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="52"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="50"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="52"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="50"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="51"/>
+      <c r="R15" s="52"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="50"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="51"/>
+      <c r="R16" s="52"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="50"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="52"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="50"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="51"/>
+      <c r="R18" s="52"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="50"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="52"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="53"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="55"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H21" s="8"/>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:18" ht="21" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="29" t="s">
         <v>143</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A23" s="40"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="55"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="55"/>
-      <c r="O23" s="55"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="55"/>
-      <c r="R23" s="41"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A24" s="42"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="56"/>
-      <c r="P24" s="56"/>
-      <c r="Q24" s="56"/>
-      <c r="R24" s="43"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A25" s="42"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="56"/>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="56"/>
-      <c r="R25" s="43"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A26" s="42"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="56"/>
-      <c r="K26" s="56"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
-      <c r="O26" s="56"/>
-      <c r="P26" s="56"/>
-      <c r="Q26" s="56"/>
-      <c r="R26" s="43"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A27" s="42"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="56"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="56"/>
-      <c r="O27" s="56"/>
-      <c r="P27" s="56"/>
-      <c r="Q27" s="56"/>
-      <c r="R27" s="43"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A28" s="42"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56"/>
-      <c r="K28" s="56"/>
-      <c r="L28" s="56"/>
-      <c r="M28" s="56"/>
-      <c r="N28" s="56"/>
-      <c r="O28" s="56"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="56"/>
-      <c r="R28" s="43"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A29" s="42"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="56"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="56"/>
-      <c r="O29" s="56"/>
-      <c r="P29" s="56"/>
-      <c r="Q29" s="56"/>
-      <c r="R29" s="43"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A30" s="42"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
-      <c r="K30" s="56"/>
-      <c r="L30" s="56"/>
-      <c r="M30" s="56"/>
-      <c r="N30" s="56"/>
-      <c r="O30" s="56"/>
-      <c r="P30" s="56"/>
-      <c r="Q30" s="56"/>
-      <c r="R30" s="43"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A31" s="42"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="43"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A32" s="42"/>
-      <c r="B32" s="56"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56"/>
-      <c r="L32" s="56"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="56"/>
-      <c r="O32" s="56"/>
-      <c r="P32" s="56"/>
-      <c r="Q32" s="56"/>
-      <c r="R32" s="43"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A33" s="42"/>
-      <c r="B33" s="56"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
-      <c r="K33" s="56"/>
-      <c r="L33" s="56"/>
-      <c r="M33" s="56"/>
-      <c r="N33" s="56"/>
-      <c r="O33" s="56"/>
-      <c r="P33" s="56"/>
-      <c r="Q33" s="56"/>
-      <c r="R33" s="43"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A34" s="42"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="56"/>
-      <c r="L34" s="56"/>
-      <c r="M34" s="56"/>
-      <c r="N34" s="56"/>
-      <c r="O34" s="56"/>
-      <c r="P34" s="56"/>
-      <c r="Q34" s="56"/>
-      <c r="R34" s="43"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A35" s="42"/>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
-      <c r="K35" s="56"/>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="56"/>
-      <c r="O35" s="56"/>
-      <c r="P35" s="56"/>
-      <c r="Q35" s="56"/>
-      <c r="R35" s="43"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A36" s="42"/>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="56"/>
-      <c r="K36" s="56"/>
-      <c r="L36" s="56"/>
-      <c r="M36" s="56"/>
-      <c r="N36" s="56"/>
-      <c r="O36" s="56"/>
-      <c r="P36" s="56"/>
-      <c r="Q36" s="56"/>
-      <c r="R36" s="43"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A37" s="42"/>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="56"/>
-      <c r="O37" s="56"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="56"/>
-      <c r="R37" s="43"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A38" s="42"/>
-      <c r="B38" s="56"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="56"/>
-      <c r="K38" s="56"/>
-      <c r="L38" s="56"/>
-      <c r="M38" s="56"/>
-      <c r="N38" s="56"/>
-      <c r="O38" s="56"/>
-      <c r="P38" s="56"/>
-      <c r="Q38" s="56"/>
-      <c r="R38" s="43"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A39" s="42"/>
-      <c r="B39" s="56"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="56"/>
-      <c r="K39" s="56"/>
-      <c r="L39" s="56"/>
-      <c r="M39" s="56"/>
-      <c r="N39" s="56"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="56"/>
-      <c r="Q39" s="56"/>
-      <c r="R39" s="43"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A40" s="42"/>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="56"/>
-      <c r="J40" s="56"/>
-      <c r="K40" s="56"/>
-      <c r="L40" s="56"/>
-      <c r="M40" s="56"/>
-      <c r="N40" s="56"/>
-      <c r="O40" s="56"/>
-      <c r="P40" s="56"/>
-      <c r="Q40" s="56"/>
-      <c r="R40" s="43"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A41" s="42"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="56"/>
-      <c r="J41" s="56"/>
-      <c r="K41" s="56"/>
-      <c r="L41" s="56"/>
-      <c r="M41" s="56"/>
-      <c r="N41" s="56"/>
-      <c r="O41" s="56"/>
-      <c r="P41" s="56"/>
-      <c r="Q41" s="56"/>
-      <c r="R41" s="43"/>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A42" s="44"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="57"/>
-      <c r="G42" s="57"/>
-      <c r="H42" s="57"/>
-      <c r="I42" s="57"/>
-      <c r="J42" s="57"/>
-      <c r="K42" s="57"/>
-      <c r="L42" s="57"/>
-      <c r="M42" s="57"/>
-      <c r="N42" s="57"/>
-      <c r="O42" s="57"/>
-      <c r="P42" s="57"/>
-      <c r="Q42" s="57"/>
-      <c r="R42" s="45"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="41"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="56"/>
+      <c r="P23" s="56"/>
+      <c r="Q23" s="56"/>
+      <c r="R23" s="42"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="43"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="57"/>
+      <c r="O24" s="57"/>
+      <c r="P24" s="57"/>
+      <c r="Q24" s="57"/>
+      <c r="R24" s="44"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="43"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="57"/>
+      <c r="P25" s="57"/>
+      <c r="Q25" s="57"/>
+      <c r="R25" s="44"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="43"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="57"/>
+      <c r="P26" s="57"/>
+      <c r="Q26" s="57"/>
+      <c r="R26" s="44"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="43"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="57"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="57"/>
+      <c r="L27" s="57"/>
+      <c r="M27" s="57"/>
+      <c r="N27" s="57"/>
+      <c r="O27" s="57"/>
+      <c r="P27" s="57"/>
+      <c r="Q27" s="57"/>
+      <c r="R27" s="44"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="43"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="57"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="57"/>
+      <c r="P28" s="57"/>
+      <c r="Q28" s="57"/>
+      <c r="R28" s="44"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="43"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="57"/>
+      <c r="M29" s="57"/>
+      <c r="N29" s="57"/>
+      <c r="O29" s="57"/>
+      <c r="P29" s="57"/>
+      <c r="Q29" s="57"/>
+      <c r="R29" s="44"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="43"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="57"/>
+      <c r="N30" s="57"/>
+      <c r="O30" s="57"/>
+      <c r="P30" s="57"/>
+      <c r="Q30" s="57"/>
+      <c r="R30" s="44"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="43"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="57"/>
+      <c r="O31" s="57"/>
+      <c r="P31" s="57"/>
+      <c r="Q31" s="57"/>
+      <c r="R31" s="44"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="43"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="57"/>
+      <c r="K32" s="57"/>
+      <c r="L32" s="57"/>
+      <c r="M32" s="57"/>
+      <c r="N32" s="57"/>
+      <c r="O32" s="57"/>
+      <c r="P32" s="57"/>
+      <c r="Q32" s="57"/>
+      <c r="R32" s="44"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="43"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="57"/>
+      <c r="I33" s="57"/>
+      <c r="J33" s="57"/>
+      <c r="K33" s="57"/>
+      <c r="L33" s="57"/>
+      <c r="M33" s="57"/>
+      <c r="N33" s="57"/>
+      <c r="O33" s="57"/>
+      <c r="P33" s="57"/>
+      <c r="Q33" s="57"/>
+      <c r="R33" s="44"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="43"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="57"/>
+      <c r="L34" s="57"/>
+      <c r="M34" s="57"/>
+      <c r="N34" s="57"/>
+      <c r="O34" s="57"/>
+      <c r="P34" s="57"/>
+      <c r="Q34" s="57"/>
+      <c r="R34" s="44"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="43"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="57"/>
+      <c r="L35" s="57"/>
+      <c r="M35" s="57"/>
+      <c r="N35" s="57"/>
+      <c r="O35" s="57"/>
+      <c r="P35" s="57"/>
+      <c r="Q35" s="57"/>
+      <c r="R35" s="44"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="57"/>
+      <c r="M36" s="57"/>
+      <c r="N36" s="57"/>
+      <c r="O36" s="57"/>
+      <c r="P36" s="57"/>
+      <c r="Q36" s="57"/>
+      <c r="R36" s="44"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="43"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
+      <c r="J37" s="57"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="57"/>
+      <c r="M37" s="57"/>
+      <c r="N37" s="57"/>
+      <c r="O37" s="57"/>
+      <c r="P37" s="57"/>
+      <c r="Q37" s="57"/>
+      <c r="R37" s="44"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="43"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="57"/>
+      <c r="K38" s="57"/>
+      <c r="L38" s="57"/>
+      <c r="M38" s="57"/>
+      <c r="N38" s="57"/>
+      <c r="O38" s="57"/>
+      <c r="P38" s="57"/>
+      <c r="Q38" s="57"/>
+      <c r="R38" s="44"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="43"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="57"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="57"/>
+      <c r="J39" s="57"/>
+      <c r="K39" s="57"/>
+      <c r="L39" s="57"/>
+      <c r="M39" s="57"/>
+      <c r="N39" s="57"/>
+      <c r="O39" s="57"/>
+      <c r="P39" s="57"/>
+      <c r="Q39" s="57"/>
+      <c r="R39" s="44"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" s="43"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="57"/>
+      <c r="H40" s="57"/>
+      <c r="I40" s="57"/>
+      <c r="J40" s="57"/>
+      <c r="K40" s="57"/>
+      <c r="L40" s="57"/>
+      <c r="M40" s="57"/>
+      <c r="N40" s="57"/>
+      <c r="O40" s="57"/>
+      <c r="P40" s="57"/>
+      <c r="Q40" s="57"/>
+      <c r="R40" s="44"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="43"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
+      <c r="J41" s="57"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="57"/>
+      <c r="M41" s="57"/>
+      <c r="N41" s="57"/>
+      <c r="O41" s="57"/>
+      <c r="P41" s="57"/>
+      <c r="Q41" s="57"/>
+      <c r="R41" s="44"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="45"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="58"/>
+      <c r="J42" s="58"/>
+      <c r="K42" s="58"/>
+      <c r="L42" s="58"/>
+      <c r="M42" s="58"/>
+      <c r="N42" s="58"/>
+      <c r="O42" s="58"/>
+      <c r="P42" s="58"/>
+      <c r="Q42" s="58"/>
+      <c r="R42" s="46"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="24"/>
       <c r="B43" s="24"/>
       <c r="C43" s="24"/>
@@ -3186,7 +3192,7 @@
       <c r="Q43" s="24"/>
       <c r="R43" s="24"/>
     </row>
-    <row r="44" spans="1:18" ht="21" x14ac:dyDescent="0.65">
+    <row r="44" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A44" s="29" t="s">
         <v>144</v>
       </c>
@@ -3208,211 +3214,211 @@
       <c r="Q44" s="24"/>
       <c r="R44" s="24"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A45" s="40"/>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="55"/>
-      <c r="L45" s="55"/>
-      <c r="M45" s="55"/>
-      <c r="N45" s="55"/>
-      <c r="O45" s="55"/>
-      <c r="P45" s="55"/>
-      <c r="Q45" s="55"/>
-      <c r="R45" s="41"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A46" s="42"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="56"/>
-      <c r="L46" s="56"/>
-      <c r="M46" s="56"/>
-      <c r="N46" s="56"/>
-      <c r="O46" s="56"/>
-      <c r="P46" s="56"/>
-      <c r="Q46" s="56"/>
-      <c r="R46" s="43"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A47" s="42"/>
-      <c r="B47" s="56"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
-      <c r="K47" s="56"/>
-      <c r="L47" s="56"/>
-      <c r="M47" s="56"/>
-      <c r="N47" s="56"/>
-      <c r="O47" s="56"/>
-      <c r="P47" s="56"/>
-      <c r="Q47" s="56"/>
-      <c r="R47" s="43"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A48" s="42"/>
-      <c r="B48" s="56"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="56"/>
-      <c r="I48" s="56"/>
-      <c r="J48" s="56"/>
-      <c r="K48" s="56"/>
-      <c r="L48" s="56"/>
-      <c r="M48" s="56"/>
-      <c r="N48" s="56"/>
-      <c r="O48" s="56"/>
-      <c r="P48" s="56"/>
-      <c r="Q48" s="56"/>
-      <c r="R48" s="43"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A49" s="42"/>
-      <c r="B49" s="56"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="56"/>
-      <c r="I49" s="56"/>
-      <c r="J49" s="56"/>
-      <c r="K49" s="56"/>
-      <c r="L49" s="56"/>
-      <c r="M49" s="56"/>
-      <c r="N49" s="56"/>
-      <c r="O49" s="56"/>
-      <c r="P49" s="56"/>
-      <c r="Q49" s="56"/>
-      <c r="R49" s="43"/>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A50" s="42"/>
-      <c r="B50" s="56"/>
-      <c r="C50" s="56"/>
-      <c r="D50" s="56"/>
-      <c r="E50" s="56"/>
-      <c r="F50" s="56"/>
-      <c r="G50" s="56"/>
-      <c r="H50" s="56"/>
-      <c r="I50" s="56"/>
-      <c r="J50" s="56"/>
-      <c r="K50" s="56"/>
-      <c r="L50" s="56"/>
-      <c r="M50" s="56"/>
-      <c r="N50" s="56"/>
-      <c r="O50" s="56"/>
-      <c r="P50" s="56"/>
-      <c r="Q50" s="56"/>
-      <c r="R50" s="43"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A51" s="42"/>
-      <c r="B51" s="56"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="56"/>
-      <c r="H51" s="56"/>
-      <c r="I51" s="56"/>
-      <c r="J51" s="56"/>
-      <c r="K51" s="56"/>
-      <c r="L51" s="56"/>
-      <c r="M51" s="56"/>
-      <c r="N51" s="56"/>
-      <c r="O51" s="56"/>
-      <c r="P51" s="56"/>
-      <c r="Q51" s="56"/>
-      <c r="R51" s="43"/>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A52" s="42"/>
-      <c r="B52" s="56"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="56"/>
-      <c r="G52" s="56"/>
-      <c r="H52" s="56"/>
-      <c r="I52" s="56"/>
-      <c r="J52" s="56"/>
-      <c r="K52" s="56"/>
-      <c r="L52" s="56"/>
-      <c r="M52" s="56"/>
-      <c r="N52" s="56"/>
-      <c r="O52" s="56"/>
-      <c r="P52" s="56"/>
-      <c r="Q52" s="56"/>
-      <c r="R52" s="43"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A53" s="42"/>
-      <c r="B53" s="56"/>
-      <c r="C53" s="56"/>
-      <c r="D53" s="56"/>
-      <c r="E53" s="56"/>
-      <c r="F53" s="56"/>
-      <c r="G53" s="56"/>
-      <c r="H53" s="56"/>
-      <c r="I53" s="56"/>
-      <c r="J53" s="56"/>
-      <c r="K53" s="56"/>
-      <c r="L53" s="56"/>
-      <c r="M53" s="56"/>
-      <c r="N53" s="56"/>
-      <c r="O53" s="56"/>
-      <c r="P53" s="56"/>
-      <c r="Q53" s="56"/>
-      <c r="R53" s="43"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A54" s="44"/>
-      <c r="B54" s="57"/>
-      <c r="C54" s="57"/>
-      <c r="D54" s="57"/>
-      <c r="E54" s="57"/>
-      <c r="F54" s="57"/>
-      <c r="G54" s="57"/>
-      <c r="H54" s="57"/>
-      <c r="I54" s="57"/>
-      <c r="J54" s="57"/>
-      <c r="K54" s="57"/>
-      <c r="L54" s="57"/>
-      <c r="M54" s="57"/>
-      <c r="N54" s="57"/>
-      <c r="O54" s="57"/>
-      <c r="P54" s="57"/>
-      <c r="Q54" s="57"/>
-      <c r="R54" s="45"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" s="41"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="56"/>
+      <c r="L45" s="56"/>
+      <c r="M45" s="56"/>
+      <c r="N45" s="56"/>
+      <c r="O45" s="56"/>
+      <c r="P45" s="56"/>
+      <c r="Q45" s="56"/>
+      <c r="R45" s="42"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" s="43"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="57"/>
+      <c r="L46" s="57"/>
+      <c r="M46" s="57"/>
+      <c r="N46" s="57"/>
+      <c r="O46" s="57"/>
+      <c r="P46" s="57"/>
+      <c r="Q46" s="57"/>
+      <c r="R46" s="44"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47" s="43"/>
+      <c r="B47" s="57"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="57"/>
+      <c r="L47" s="57"/>
+      <c r="M47" s="57"/>
+      <c r="N47" s="57"/>
+      <c r="O47" s="57"/>
+      <c r="P47" s="57"/>
+      <c r="Q47" s="57"/>
+      <c r="R47" s="44"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48" s="43"/>
+      <c r="B48" s="57"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="57"/>
+      <c r="J48" s="57"/>
+      <c r="K48" s="57"/>
+      <c r="L48" s="57"/>
+      <c r="M48" s="57"/>
+      <c r="N48" s="57"/>
+      <c r="O48" s="57"/>
+      <c r="P48" s="57"/>
+      <c r="Q48" s="57"/>
+      <c r="R48" s="44"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49" s="43"/>
+      <c r="B49" s="57"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="57"/>
+      <c r="J49" s="57"/>
+      <c r="K49" s="57"/>
+      <c r="L49" s="57"/>
+      <c r="M49" s="57"/>
+      <c r="N49" s="57"/>
+      <c r="O49" s="57"/>
+      <c r="P49" s="57"/>
+      <c r="Q49" s="57"/>
+      <c r="R49" s="44"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" s="43"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
+      <c r="L50" s="57"/>
+      <c r="M50" s="57"/>
+      <c r="N50" s="57"/>
+      <c r="O50" s="57"/>
+      <c r="P50" s="57"/>
+      <c r="Q50" s="57"/>
+      <c r="R50" s="44"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51" s="43"/>
+      <c r="B51" s="57"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="57"/>
+      <c r="L51" s="57"/>
+      <c r="M51" s="57"/>
+      <c r="N51" s="57"/>
+      <c r="O51" s="57"/>
+      <c r="P51" s="57"/>
+      <c r="Q51" s="57"/>
+      <c r="R51" s="44"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" s="43"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="57"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="57"/>
+      <c r="L52" s="57"/>
+      <c r="M52" s="57"/>
+      <c r="N52" s="57"/>
+      <c r="O52" s="57"/>
+      <c r="P52" s="57"/>
+      <c r="Q52" s="57"/>
+      <c r="R52" s="44"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53" s="43"/>
+      <c r="B53" s="57"/>
+      <c r="C53" s="57"/>
+      <c r="D53" s="57"/>
+      <c r="E53" s="57"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="57"/>
+      <c r="J53" s="57"/>
+      <c r="K53" s="57"/>
+      <c r="L53" s="57"/>
+      <c r="M53" s="57"/>
+      <c r="N53" s="57"/>
+      <c r="O53" s="57"/>
+      <c r="P53" s="57"/>
+      <c r="Q53" s="57"/>
+      <c r="R53" s="44"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" s="45"/>
+      <c r="B54" s="58"/>
+      <c r="C54" s="58"/>
+      <c r="D54" s="58"/>
+      <c r="E54" s="58"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="58"/>
+      <c r="J54" s="58"/>
+      <c r="K54" s="58"/>
+      <c r="L54" s="58"/>
+      <c r="M54" s="58"/>
+      <c r="N54" s="58"/>
+      <c r="O54" s="58"/>
+      <c r="P54" s="58"/>
+      <c r="Q54" s="58"/>
+      <c r="R54" s="46"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H55" s="8"/>
       <c r="I55" s="5"/>
     </row>
-    <row r="56" spans="1:18" ht="21" x14ac:dyDescent="0.65">
+    <row r="56" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A56" s="29" t="s">
         <v>145</v>
       </c>
@@ -3434,219 +3440,219 @@
       <c r="Q56" s="24"/>
       <c r="R56" s="24"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A57" s="40"/>
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="55"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="55"/>
-      <c r="G57" s="55"/>
-      <c r="H57" s="55"/>
-      <c r="I57" s="55"/>
-      <c r="J57" s="55"/>
-      <c r="K57" s="55"/>
-      <c r="L57" s="55"/>
-      <c r="M57" s="55"/>
-      <c r="N57" s="55"/>
-      <c r="O57" s="55"/>
-      <c r="P57" s="55"/>
-      <c r="Q57" s="55"/>
-      <c r="R57" s="41"/>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A58" s="42"/>
-      <c r="B58" s="56"/>
-      <c r="C58" s="56"/>
-      <c r="D58" s="56"/>
-      <c r="E58" s="56"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="56"/>
-      <c r="H58" s="56"/>
-      <c r="I58" s="56"/>
-      <c r="J58" s="56"/>
-      <c r="K58" s="56"/>
-      <c r="L58" s="56"/>
-      <c r="M58" s="56"/>
-      <c r="N58" s="56"/>
-      <c r="O58" s="56"/>
-      <c r="P58" s="56"/>
-      <c r="Q58" s="56"/>
-      <c r="R58" s="43"/>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A59" s="42"/>
-      <c r="B59" s="56"/>
-      <c r="C59" s="56"/>
-      <c r="D59" s="56"/>
-      <c r="E59" s="56"/>
-      <c r="F59" s="56"/>
-      <c r="G59" s="56"/>
-      <c r="H59" s="56"/>
-      <c r="I59" s="56"/>
-      <c r="J59" s="56"/>
-      <c r="K59" s="56"/>
-      <c r="L59" s="56"/>
-      <c r="M59" s="56"/>
-      <c r="N59" s="56"/>
-      <c r="O59" s="56"/>
-      <c r="P59" s="56"/>
-      <c r="Q59" s="56"/>
-      <c r="R59" s="43"/>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A60" s="42"/>
-      <c r="B60" s="56"/>
-      <c r="C60" s="56"/>
-      <c r="D60" s="56"/>
-      <c r="E60" s="56"/>
-      <c r="F60" s="56"/>
-      <c r="G60" s="56"/>
-      <c r="H60" s="56"/>
-      <c r="I60" s="56"/>
-      <c r="J60" s="56"/>
-      <c r="K60" s="56"/>
-      <c r="L60" s="56"/>
-      <c r="M60" s="56"/>
-      <c r="N60" s="56"/>
-      <c r="O60" s="56"/>
-      <c r="P60" s="56"/>
-      <c r="Q60" s="56"/>
-      <c r="R60" s="43"/>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A61" s="42"/>
-      <c r="B61" s="56"/>
-      <c r="C61" s="56"/>
-      <c r="D61" s="56"/>
-      <c r="E61" s="56"/>
-      <c r="F61" s="56"/>
-      <c r="G61" s="56"/>
-      <c r="H61" s="56"/>
-      <c r="I61" s="56"/>
-      <c r="J61" s="56"/>
-      <c r="K61" s="56"/>
-      <c r="L61" s="56"/>
-      <c r="M61" s="56"/>
-      <c r="N61" s="56"/>
-      <c r="O61" s="56"/>
-      <c r="P61" s="56"/>
-      <c r="Q61" s="56"/>
-      <c r="R61" s="43"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A62" s="42"/>
-      <c r="B62" s="56"/>
-      <c r="C62" s="56"/>
-      <c r="D62" s="56"/>
-      <c r="E62" s="56"/>
-      <c r="F62" s="56"/>
-      <c r="G62" s="56"/>
-      <c r="H62" s="56"/>
-      <c r="I62" s="56"/>
-      <c r="J62" s="56"/>
-      <c r="K62" s="56"/>
-      <c r="L62" s="56"/>
-      <c r="M62" s="56"/>
-      <c r="N62" s="56"/>
-      <c r="O62" s="56"/>
-      <c r="P62" s="56"/>
-      <c r="Q62" s="56"/>
-      <c r="R62" s="43"/>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A63" s="42"/>
-      <c r="B63" s="56"/>
-      <c r="C63" s="56"/>
-      <c r="D63" s="56"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56"/>
-      <c r="H63" s="56"/>
-      <c r="I63" s="56"/>
-      <c r="J63" s="56"/>
-      <c r="K63" s="56"/>
-      <c r="L63" s="56"/>
-      <c r="M63" s="56"/>
-      <c r="N63" s="56"/>
-      <c r="O63" s="56"/>
-      <c r="P63" s="56"/>
-      <c r="Q63" s="56"/>
-      <c r="R63" s="43"/>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A64" s="42"/>
-      <c r="B64" s="56"/>
-      <c r="C64" s="56"/>
-      <c r="D64" s="56"/>
-      <c r="E64" s="56"/>
-      <c r="F64" s="56"/>
-      <c r="G64" s="56"/>
-      <c r="H64" s="56"/>
-      <c r="I64" s="56"/>
-      <c r="J64" s="56"/>
-      <c r="K64" s="56"/>
-      <c r="L64" s="56"/>
-      <c r="M64" s="56"/>
-      <c r="N64" s="56"/>
-      <c r="O64" s="56"/>
-      <c r="P64" s="56"/>
-      <c r="Q64" s="56"/>
-      <c r="R64" s="43"/>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A65" s="42"/>
-      <c r="B65" s="56"/>
-      <c r="C65" s="56"/>
-      <c r="D65" s="56"/>
-      <c r="E65" s="56"/>
-      <c r="F65" s="56"/>
-      <c r="G65" s="56"/>
-      <c r="H65" s="56"/>
-      <c r="I65" s="56"/>
-      <c r="J65" s="56"/>
-      <c r="K65" s="56"/>
-      <c r="L65" s="56"/>
-      <c r="M65" s="56"/>
-      <c r="N65" s="56"/>
-      <c r="O65" s="56"/>
-      <c r="P65" s="56"/>
-      <c r="Q65" s="56"/>
-      <c r="R65" s="43"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A66" s="44"/>
-      <c r="B66" s="57"/>
-      <c r="C66" s="57"/>
-      <c r="D66" s="57"/>
-      <c r="E66" s="57"/>
-      <c r="F66" s="57"/>
-      <c r="G66" s="57"/>
-      <c r="H66" s="57"/>
-      <c r="I66" s="57"/>
-      <c r="J66" s="57"/>
-      <c r="K66" s="57"/>
-      <c r="L66" s="57"/>
-      <c r="M66" s="57"/>
-      <c r="N66" s="57"/>
-      <c r="O66" s="57"/>
-      <c r="P66" s="57"/>
-      <c r="Q66" s="57"/>
-      <c r="R66" s="45"/>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" s="41"/>
+      <c r="B57" s="56"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="56"/>
+      <c r="E57" s="56"/>
+      <c r="F57" s="56"/>
+      <c r="G57" s="56"/>
+      <c r="H57" s="56"/>
+      <c r="I57" s="56"/>
+      <c r="J57" s="56"/>
+      <c r="K57" s="56"/>
+      <c r="L57" s="56"/>
+      <c r="M57" s="56"/>
+      <c r="N57" s="56"/>
+      <c r="O57" s="56"/>
+      <c r="P57" s="56"/>
+      <c r="Q57" s="56"/>
+      <c r="R57" s="42"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" s="43"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="57"/>
+      <c r="E58" s="57"/>
+      <c r="F58" s="57"/>
+      <c r="G58" s="57"/>
+      <c r="H58" s="57"/>
+      <c r="I58" s="57"/>
+      <c r="J58" s="57"/>
+      <c r="K58" s="57"/>
+      <c r="L58" s="57"/>
+      <c r="M58" s="57"/>
+      <c r="N58" s="57"/>
+      <c r="O58" s="57"/>
+      <c r="P58" s="57"/>
+      <c r="Q58" s="57"/>
+      <c r="R58" s="44"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59" s="43"/>
+      <c r="B59" s="57"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
+      <c r="E59" s="57"/>
+      <c r="F59" s="57"/>
+      <c r="G59" s="57"/>
+      <c r="H59" s="57"/>
+      <c r="I59" s="57"/>
+      <c r="J59" s="57"/>
+      <c r="K59" s="57"/>
+      <c r="L59" s="57"/>
+      <c r="M59" s="57"/>
+      <c r="N59" s="57"/>
+      <c r="O59" s="57"/>
+      <c r="P59" s="57"/>
+      <c r="Q59" s="57"/>
+      <c r="R59" s="44"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60" s="43"/>
+      <c r="B60" s="57"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="57"/>
+      <c r="F60" s="57"/>
+      <c r="G60" s="57"/>
+      <c r="H60" s="57"/>
+      <c r="I60" s="57"/>
+      <c r="J60" s="57"/>
+      <c r="K60" s="57"/>
+      <c r="L60" s="57"/>
+      <c r="M60" s="57"/>
+      <c r="N60" s="57"/>
+      <c r="O60" s="57"/>
+      <c r="P60" s="57"/>
+      <c r="Q60" s="57"/>
+      <c r="R60" s="44"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" s="43"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="57"/>
+      <c r="F61" s="57"/>
+      <c r="G61" s="57"/>
+      <c r="H61" s="57"/>
+      <c r="I61" s="57"/>
+      <c r="J61" s="57"/>
+      <c r="K61" s="57"/>
+      <c r="L61" s="57"/>
+      <c r="M61" s="57"/>
+      <c r="N61" s="57"/>
+      <c r="O61" s="57"/>
+      <c r="P61" s="57"/>
+      <c r="Q61" s="57"/>
+      <c r="R61" s="44"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" s="43"/>
+      <c r="B62" s="57"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="57"/>
+      <c r="F62" s="57"/>
+      <c r="G62" s="57"/>
+      <c r="H62" s="57"/>
+      <c r="I62" s="57"/>
+      <c r="J62" s="57"/>
+      <c r="K62" s="57"/>
+      <c r="L62" s="57"/>
+      <c r="M62" s="57"/>
+      <c r="N62" s="57"/>
+      <c r="O62" s="57"/>
+      <c r="P62" s="57"/>
+      <c r="Q62" s="57"/>
+      <c r="R62" s="44"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63" s="43"/>
+      <c r="B63" s="57"/>
+      <c r="C63" s="57"/>
+      <c r="D63" s="57"/>
+      <c r="E63" s="57"/>
+      <c r="F63" s="57"/>
+      <c r="G63" s="57"/>
+      <c r="H63" s="57"/>
+      <c r="I63" s="57"/>
+      <c r="J63" s="57"/>
+      <c r="K63" s="57"/>
+      <c r="L63" s="57"/>
+      <c r="M63" s="57"/>
+      <c r="N63" s="57"/>
+      <c r="O63" s="57"/>
+      <c r="P63" s="57"/>
+      <c r="Q63" s="57"/>
+      <c r="R63" s="44"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A64" s="43"/>
+      <c r="B64" s="57"/>
+      <c r="C64" s="57"/>
+      <c r="D64" s="57"/>
+      <c r="E64" s="57"/>
+      <c r="F64" s="57"/>
+      <c r="G64" s="57"/>
+      <c r="H64" s="57"/>
+      <c r="I64" s="57"/>
+      <c r="J64" s="57"/>
+      <c r="K64" s="57"/>
+      <c r="L64" s="57"/>
+      <c r="M64" s="57"/>
+      <c r="N64" s="57"/>
+      <c r="O64" s="57"/>
+      <c r="P64" s="57"/>
+      <c r="Q64" s="57"/>
+      <c r="R64" s="44"/>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" s="43"/>
+      <c r="B65" s="57"/>
+      <c r="C65" s="57"/>
+      <c r="D65" s="57"/>
+      <c r="E65" s="57"/>
+      <c r="F65" s="57"/>
+      <c r="G65" s="57"/>
+      <c r="H65" s="57"/>
+      <c r="I65" s="57"/>
+      <c r="J65" s="57"/>
+      <c r="K65" s="57"/>
+      <c r="L65" s="57"/>
+      <c r="M65" s="57"/>
+      <c r="N65" s="57"/>
+      <c r="O65" s="57"/>
+      <c r="P65" s="57"/>
+      <c r="Q65" s="57"/>
+      <c r="R65" s="44"/>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" s="45"/>
+      <c r="B66" s="58"/>
+      <c r="C66" s="58"/>
+      <c r="D66" s="58"/>
+      <c r="E66" s="58"/>
+      <c r="F66" s="58"/>
+      <c r="G66" s="58"/>
+      <c r="H66" s="58"/>
+      <c r="I66" s="58"/>
+      <c r="J66" s="58"/>
+      <c r="K66" s="58"/>
+      <c r="L66" s="58"/>
+      <c r="M66" s="58"/>
+      <c r="N66" s="58"/>
+      <c r="O66" s="58"/>
+      <c r="P66" s="58"/>
+      <c r="Q66" s="58"/>
+      <c r="R66" s="46"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H67" s="8"/>
       <c r="I67" s="5"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H68" s="8"/>
       <c r="I68" s="5"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H69" s="8"/>
       <c r="I69" s="5"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H70" s="8"/>
       <c r="I70" s="5"/>
     </row>

</xml_diff>

<commit_message>
Created a model report and some tests to demonstrate how to create a report
</commit_message>
<xml_diff>
--- a/Src/SummitReports.Objects/Reports/UWRelationshipCashFlowReport/UW-RCF-Reports.xlsx
+++ b/Src/SummitReports.Objects/Reports/UWRelationshipCashFlowReport/UW-RCF-Reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Summit\SummitReports\Src\SummitReports.Objects\Reports\UWRelationshipCashFlowReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C46BE03-0899-4860-B463-6B92120336B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F0D1FE-D0AA-41D1-9959-AEA120B11DE7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1885,11 +1885,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8FA40D-F3F7-4105-8B77-A0262887423C}">
-  <sheetPr codeName="Sheet3"/>
+  <sheetPr codeName="Sheet3">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A2:S17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,6 +2109,17 @@
       <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="38" t="str">
+        <f>RelationshipData!X1</f>
+        <v>36 hole mini golf course and race track</v>
+      </c>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="39"/>
       <c r="H8"/>
       <c r="I8" s="18"/>
       <c r="M8" s="11" t="s">
@@ -2123,16 +2136,6 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="38" t="str">
-        <f>RelationshipData!X1</f>
-        <v>36 hole mini golf course and race track</v>
-      </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="39"/>
       <c r="H9" s="8" t="s">
         <v>106</v>
       </c>
@@ -2355,33 +2358,36 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B9:E9"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="E11:F14"/>
+    <mergeCell ref="B8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup scale="35" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5FA1A1-6E42-405D-B2DA-0D63F2AF1F86}">
-  <dimension ref="A1:R70"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:R66"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
         <v>142</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="47"/>
       <c r="B2" s="48"/>
       <c r="C2" s="48"/>
@@ -2399,9 +2405,17 @@
       <c r="O2" s="48"/>
       <c r="P2" s="48"/>
       <c r="Q2" s="48"/>
-      <c r="R2" s="49"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="49"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="50"/>
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
@@ -2419,9 +2433,17 @@
       <c r="O3" s="51"/>
       <c r="P3" s="51"/>
       <c r="Q3" s="51"/>
-      <c r="R3" s="52"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+      <c r="T3" s="51"/>
+      <c r="U3" s="51"/>
+      <c r="V3" s="51"/>
+      <c r="W3" s="51"/>
+      <c r="X3" s="51"/>
+      <c r="Y3" s="51"/>
+      <c r="Z3" s="52"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="50"/>
       <c r="B4" s="51"/>
       <c r="C4" s="51"/>
@@ -2439,9 +2461,17 @@
       <c r="O4" s="51"/>
       <c r="P4" s="51"/>
       <c r="Q4" s="51"/>
-      <c r="R4" s="52"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
+      <c r="T4" s="51"/>
+      <c r="U4" s="51"/>
+      <c r="V4" s="51"/>
+      <c r="W4" s="51"/>
+      <c r="X4" s="51"/>
+      <c r="Y4" s="51"/>
+      <c r="Z4" s="52"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="50"/>
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
@@ -2459,9 +2489,17 @@
       <c r="O5" s="51"/>
       <c r="P5" s="51"/>
       <c r="Q5" s="51"/>
-      <c r="R5" s="52"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="51"/>
+      <c r="W5" s="51"/>
+      <c r="X5" s="51"/>
+      <c r="Y5" s="51"/>
+      <c r="Z5" s="52"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="50"/>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
@@ -2479,9 +2517,17 @@
       <c r="O6" s="51"/>
       <c r="P6" s="51"/>
       <c r="Q6" s="51"/>
-      <c r="R6" s="52"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R6" s="51"/>
+      <c r="S6" s="51"/>
+      <c r="T6" s="51"/>
+      <c r="U6" s="51"/>
+      <c r="V6" s="51"/>
+      <c r="W6" s="51"/>
+      <c r="X6" s="51"/>
+      <c r="Y6" s="51"/>
+      <c r="Z6" s="52"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="50"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
@@ -2499,9 +2545,17 @@
       <c r="O7" s="51"/>
       <c r="P7" s="51"/>
       <c r="Q7" s="51"/>
-      <c r="R7" s="52"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R7" s="51"/>
+      <c r="S7" s="51"/>
+      <c r="T7" s="51"/>
+      <c r="U7" s="51"/>
+      <c r="V7" s="51"/>
+      <c r="W7" s="51"/>
+      <c r="X7" s="51"/>
+      <c r="Y7" s="51"/>
+      <c r="Z7" s="52"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="50"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -2519,9 +2573,17 @@
       <c r="O8" s="51"/>
       <c r="P8" s="51"/>
       <c r="Q8" s="51"/>
-      <c r="R8" s="52"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="51"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="51"/>
+      <c r="X8" s="51"/>
+      <c r="Y8" s="51"/>
+      <c r="Z8" s="52"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="50"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -2539,9 +2601,17 @@
       <c r="O9" s="51"/>
       <c r="P9" s="51"/>
       <c r="Q9" s="51"/>
-      <c r="R9" s="52"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R9" s="51"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="51"/>
+      <c r="U9" s="51"/>
+      <c r="V9" s="51"/>
+      <c r="W9" s="51"/>
+      <c r="X9" s="51"/>
+      <c r="Y9" s="51"/>
+      <c r="Z9" s="52"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="50"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -2559,9 +2629,17 @@
       <c r="O10" s="51"/>
       <c r="P10" s="51"/>
       <c r="Q10" s="51"/>
-      <c r="R10" s="52"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R10" s="51"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="51"/>
+      <c r="U10" s="51"/>
+      <c r="V10" s="51"/>
+      <c r="W10" s="51"/>
+      <c r="X10" s="51"/>
+      <c r="Y10" s="51"/>
+      <c r="Z10" s="52"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="50"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -2579,9 +2657,17 @@
       <c r="O11" s="51"/>
       <c r="P11" s="51"/>
       <c r="Q11" s="51"/>
-      <c r="R11" s="52"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R11" s="51"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="51"/>
+      <c r="U11" s="51"/>
+      <c r="V11" s="51"/>
+      <c r="W11" s="51"/>
+      <c r="X11" s="51"/>
+      <c r="Y11" s="51"/>
+      <c r="Z11" s="52"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="50"/>
       <c r="B12" s="51"/>
       <c r="C12" s="51"/>
@@ -2599,9 +2685,17 @@
       <c r="O12" s="51"/>
       <c r="P12" s="51"/>
       <c r="Q12" s="51"/>
-      <c r="R12" s="52"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R12" s="51"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="51"/>
+      <c r="U12" s="51"/>
+      <c r="V12" s="51"/>
+      <c r="W12" s="51"/>
+      <c r="X12" s="51"/>
+      <c r="Y12" s="51"/>
+      <c r="Z12" s="52"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="50"/>
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
@@ -2619,9 +2713,17 @@
       <c r="O13" s="51"/>
       <c r="P13" s="51"/>
       <c r="Q13" s="51"/>
-      <c r="R13" s="52"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R13" s="51"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="51"/>
+      <c r="U13" s="51"/>
+      <c r="V13" s="51"/>
+      <c r="W13" s="51"/>
+      <c r="X13" s="51"/>
+      <c r="Y13" s="51"/>
+      <c r="Z13" s="52"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="50"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
@@ -2639,9 +2741,17 @@
       <c r="O14" s="51"/>
       <c r="P14" s="51"/>
       <c r="Q14" s="51"/>
-      <c r="R14" s="52"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="51"/>
+      <c r="Z14" s="52"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="50"/>
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
@@ -2659,9 +2769,17 @@
       <c r="O15" s="51"/>
       <c r="P15" s="51"/>
       <c r="Q15" s="51"/>
-      <c r="R15" s="52"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R15" s="51"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="51"/>
+      <c r="U15" s="51"/>
+      <c r="V15" s="51"/>
+      <c r="W15" s="51"/>
+      <c r="X15" s="51"/>
+      <c r="Y15" s="51"/>
+      <c r="Z15" s="52"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="50"/>
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
@@ -2679,9 +2797,17 @@
       <c r="O16" s="51"/>
       <c r="P16" s="51"/>
       <c r="Q16" s="51"/>
-      <c r="R16" s="52"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R16" s="51"/>
+      <c r="S16" s="51"/>
+      <c r="T16" s="51"/>
+      <c r="U16" s="51"/>
+      <c r="V16" s="51"/>
+      <c r="W16" s="51"/>
+      <c r="X16" s="51"/>
+      <c r="Y16" s="51"/>
+      <c r="Z16" s="52"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="50"/>
       <c r="B17" s="51"/>
       <c r="C17" s="51"/>
@@ -2699,9 +2825,17 @@
       <c r="O17" s="51"/>
       <c r="P17" s="51"/>
       <c r="Q17" s="51"/>
-      <c r="R17" s="52"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R17" s="51"/>
+      <c r="S17" s="51"/>
+      <c r="T17" s="51"/>
+      <c r="U17" s="51"/>
+      <c r="V17" s="51"/>
+      <c r="W17" s="51"/>
+      <c r="X17" s="51"/>
+      <c r="Y17" s="51"/>
+      <c r="Z17" s="52"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="50"/>
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
@@ -2719,9 +2853,17 @@
       <c r="O18" s="51"/>
       <c r="P18" s="51"/>
       <c r="Q18" s="51"/>
-      <c r="R18" s="52"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R18" s="51"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="51"/>
+      <c r="Y18" s="51"/>
+      <c r="Z18" s="52"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="50"/>
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
@@ -2739,9 +2881,17 @@
       <c r="O19" s="51"/>
       <c r="P19" s="51"/>
       <c r="Q19" s="51"/>
-      <c r="R19" s="52"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R19" s="51"/>
+      <c r="S19" s="51"/>
+      <c r="T19" s="51"/>
+      <c r="U19" s="51"/>
+      <c r="V19" s="51"/>
+      <c r="W19" s="51"/>
+      <c r="X19" s="51"/>
+      <c r="Y19" s="51"/>
+      <c r="Z19" s="52"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="53"/>
       <c r="B20" s="54"/>
       <c r="C20" s="54"/>
@@ -2759,20 +2909,28 @@
       <c r="O20" s="54"/>
       <c r="P20" s="54"/>
       <c r="Q20" s="54"/>
-      <c r="R20" s="55"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R20" s="54"/>
+      <c r="S20" s="54"/>
+      <c r="T20" s="54"/>
+      <c r="U20" s="54"/>
+      <c r="V20" s="54"/>
+      <c r="W20" s="54"/>
+      <c r="X20" s="54"/>
+      <c r="Y20" s="54"/>
+      <c r="Z20" s="55"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H21" s="8"/>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="29" t="s">
         <v>143</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="41"/>
       <c r="B23" s="56"/>
       <c r="C23" s="56"/>
@@ -2790,9 +2948,17 @@
       <c r="O23" s="56"/>
       <c r="P23" s="56"/>
       <c r="Q23" s="56"/>
-      <c r="R23" s="42"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R23" s="56"/>
+      <c r="S23" s="56"/>
+      <c r="T23" s="56"/>
+      <c r="U23" s="56"/>
+      <c r="V23" s="56"/>
+      <c r="W23" s="56"/>
+      <c r="X23" s="56"/>
+      <c r="Y23" s="56"/>
+      <c r="Z23" s="42"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="43"/>
       <c r="B24" s="57"/>
       <c r="C24" s="57"/>
@@ -2810,9 +2976,17 @@
       <c r="O24" s="57"/>
       <c r="P24" s="57"/>
       <c r="Q24" s="57"/>
-      <c r="R24" s="44"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R24" s="57"/>
+      <c r="S24" s="57"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="57"/>
+      <c r="V24" s="57"/>
+      <c r="W24" s="57"/>
+      <c r="X24" s="57"/>
+      <c r="Y24" s="57"/>
+      <c r="Z24" s="44"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="43"/>
       <c r="B25" s="57"/>
       <c r="C25" s="57"/>
@@ -2830,9 +3004,17 @@
       <c r="O25" s="57"/>
       <c r="P25" s="57"/>
       <c r="Q25" s="57"/>
-      <c r="R25" s="44"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R25" s="57"/>
+      <c r="S25" s="57"/>
+      <c r="T25" s="57"/>
+      <c r="U25" s="57"/>
+      <c r="V25" s="57"/>
+      <c r="W25" s="57"/>
+      <c r="X25" s="57"/>
+      <c r="Y25" s="57"/>
+      <c r="Z25" s="44"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="43"/>
       <c r="B26" s="57"/>
       <c r="C26" s="57"/>
@@ -2850,9 +3032,17 @@
       <c r="O26" s="57"/>
       <c r="P26" s="57"/>
       <c r="Q26" s="57"/>
-      <c r="R26" s="44"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R26" s="57"/>
+      <c r="S26" s="57"/>
+      <c r="T26" s="57"/>
+      <c r="U26" s="57"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="57"/>
+      <c r="X26" s="57"/>
+      <c r="Y26" s="57"/>
+      <c r="Z26" s="44"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="43"/>
       <c r="B27" s="57"/>
       <c r="C27" s="57"/>
@@ -2870,9 +3060,17 @@
       <c r="O27" s="57"/>
       <c r="P27" s="57"/>
       <c r="Q27" s="57"/>
-      <c r="R27" s="44"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R27" s="57"/>
+      <c r="S27" s="57"/>
+      <c r="T27" s="57"/>
+      <c r="U27" s="57"/>
+      <c r="V27" s="57"/>
+      <c r="W27" s="57"/>
+      <c r="X27" s="57"/>
+      <c r="Y27" s="57"/>
+      <c r="Z27" s="44"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="43"/>
       <c r="B28" s="57"/>
       <c r="C28" s="57"/>
@@ -2890,9 +3088,17 @@
       <c r="O28" s="57"/>
       <c r="P28" s="57"/>
       <c r="Q28" s="57"/>
-      <c r="R28" s="44"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R28" s="57"/>
+      <c r="S28" s="57"/>
+      <c r="T28" s="57"/>
+      <c r="U28" s="57"/>
+      <c r="V28" s="57"/>
+      <c r="W28" s="57"/>
+      <c r="X28" s="57"/>
+      <c r="Y28" s="57"/>
+      <c r="Z28" s="44"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="43"/>
       <c r="B29" s="57"/>
       <c r="C29" s="57"/>
@@ -2910,9 +3116,17 @@
       <c r="O29" s="57"/>
       <c r="P29" s="57"/>
       <c r="Q29" s="57"/>
-      <c r="R29" s="44"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R29" s="57"/>
+      <c r="S29" s="57"/>
+      <c r="T29" s="57"/>
+      <c r="U29" s="57"/>
+      <c r="V29" s="57"/>
+      <c r="W29" s="57"/>
+      <c r="X29" s="57"/>
+      <c r="Y29" s="57"/>
+      <c r="Z29" s="44"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="43"/>
       <c r="B30" s="57"/>
       <c r="C30" s="57"/>
@@ -2930,9 +3144,17 @@
       <c r="O30" s="57"/>
       <c r="P30" s="57"/>
       <c r="Q30" s="57"/>
-      <c r="R30" s="44"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R30" s="57"/>
+      <c r="S30" s="57"/>
+      <c r="T30" s="57"/>
+      <c r="U30" s="57"/>
+      <c r="V30" s="57"/>
+      <c r="W30" s="57"/>
+      <c r="X30" s="57"/>
+      <c r="Y30" s="57"/>
+      <c r="Z30" s="44"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="43"/>
       <c r="B31" s="57"/>
       <c r="C31" s="57"/>
@@ -2950,9 +3172,17 @@
       <c r="O31" s="57"/>
       <c r="P31" s="57"/>
       <c r="Q31" s="57"/>
-      <c r="R31" s="44"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R31" s="57"/>
+      <c r="S31" s="57"/>
+      <c r="T31" s="57"/>
+      <c r="U31" s="57"/>
+      <c r="V31" s="57"/>
+      <c r="W31" s="57"/>
+      <c r="X31" s="57"/>
+      <c r="Y31" s="57"/>
+      <c r="Z31" s="44"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="43"/>
       <c r="B32" s="57"/>
       <c r="C32" s="57"/>
@@ -2970,9 +3200,17 @@
       <c r="O32" s="57"/>
       <c r="P32" s="57"/>
       <c r="Q32" s="57"/>
-      <c r="R32" s="44"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R32" s="57"/>
+      <c r="S32" s="57"/>
+      <c r="T32" s="57"/>
+      <c r="U32" s="57"/>
+      <c r="V32" s="57"/>
+      <c r="W32" s="57"/>
+      <c r="X32" s="57"/>
+      <c r="Y32" s="57"/>
+      <c r="Z32" s="44"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="43"/>
       <c r="B33" s="57"/>
       <c r="C33" s="57"/>
@@ -2990,9 +3228,17 @@
       <c r="O33" s="57"/>
       <c r="P33" s="57"/>
       <c r="Q33" s="57"/>
-      <c r="R33" s="44"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R33" s="57"/>
+      <c r="S33" s="57"/>
+      <c r="T33" s="57"/>
+      <c r="U33" s="57"/>
+      <c r="V33" s="57"/>
+      <c r="W33" s="57"/>
+      <c r="X33" s="57"/>
+      <c r="Y33" s="57"/>
+      <c r="Z33" s="44"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="43"/>
       <c r="B34" s="57"/>
       <c r="C34" s="57"/>
@@ -3010,9 +3256,17 @@
       <c r="O34" s="57"/>
       <c r="P34" s="57"/>
       <c r="Q34" s="57"/>
-      <c r="R34" s="44"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R34" s="57"/>
+      <c r="S34" s="57"/>
+      <c r="T34" s="57"/>
+      <c r="U34" s="57"/>
+      <c r="V34" s="57"/>
+      <c r="W34" s="57"/>
+      <c r="X34" s="57"/>
+      <c r="Y34" s="57"/>
+      <c r="Z34" s="44"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="43"/>
       <c r="B35" s="57"/>
       <c r="C35" s="57"/>
@@ -3030,9 +3284,17 @@
       <c r="O35" s="57"/>
       <c r="P35" s="57"/>
       <c r="Q35" s="57"/>
-      <c r="R35" s="44"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R35" s="57"/>
+      <c r="S35" s="57"/>
+      <c r="T35" s="57"/>
+      <c r="U35" s="57"/>
+      <c r="V35" s="57"/>
+      <c r="W35" s="57"/>
+      <c r="X35" s="57"/>
+      <c r="Y35" s="57"/>
+      <c r="Z35" s="44"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="43"/>
       <c r="B36" s="57"/>
       <c r="C36" s="57"/>
@@ -3050,9 +3312,17 @@
       <c r="O36" s="57"/>
       <c r="P36" s="57"/>
       <c r="Q36" s="57"/>
-      <c r="R36" s="44"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R36" s="57"/>
+      <c r="S36" s="57"/>
+      <c r="T36" s="57"/>
+      <c r="U36" s="57"/>
+      <c r="V36" s="57"/>
+      <c r="W36" s="57"/>
+      <c r="X36" s="57"/>
+      <c r="Y36" s="57"/>
+      <c r="Z36" s="44"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="43"/>
       <c r="B37" s="57"/>
       <c r="C37" s="57"/>
@@ -3070,9 +3340,17 @@
       <c r="O37" s="57"/>
       <c r="P37" s="57"/>
       <c r="Q37" s="57"/>
-      <c r="R37" s="44"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R37" s="57"/>
+      <c r="S37" s="57"/>
+      <c r="T37" s="57"/>
+      <c r="U37" s="57"/>
+      <c r="V37" s="57"/>
+      <c r="W37" s="57"/>
+      <c r="X37" s="57"/>
+      <c r="Y37" s="57"/>
+      <c r="Z37" s="44"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="43"/>
       <c r="B38" s="57"/>
       <c r="C38" s="57"/>
@@ -3090,9 +3368,17 @@
       <c r="O38" s="57"/>
       <c r="P38" s="57"/>
       <c r="Q38" s="57"/>
-      <c r="R38" s="44"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R38" s="57"/>
+      <c r="S38" s="57"/>
+      <c r="T38" s="57"/>
+      <c r="U38" s="57"/>
+      <c r="V38" s="57"/>
+      <c r="W38" s="57"/>
+      <c r="X38" s="57"/>
+      <c r="Y38" s="57"/>
+      <c r="Z38" s="44"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="43"/>
       <c r="B39" s="57"/>
       <c r="C39" s="57"/>
@@ -3110,9 +3396,17 @@
       <c r="O39" s="57"/>
       <c r="P39" s="57"/>
       <c r="Q39" s="57"/>
-      <c r="R39" s="44"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R39" s="57"/>
+      <c r="S39" s="57"/>
+      <c r="T39" s="57"/>
+      <c r="U39" s="57"/>
+      <c r="V39" s="57"/>
+      <c r="W39" s="57"/>
+      <c r="X39" s="57"/>
+      <c r="Y39" s="57"/>
+      <c r="Z39" s="44"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="43"/>
       <c r="B40" s="57"/>
       <c r="C40" s="57"/>
@@ -3130,9 +3424,17 @@
       <c r="O40" s="57"/>
       <c r="P40" s="57"/>
       <c r="Q40" s="57"/>
-      <c r="R40" s="44"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R40" s="57"/>
+      <c r="S40" s="57"/>
+      <c r="T40" s="57"/>
+      <c r="U40" s="57"/>
+      <c r="V40" s="57"/>
+      <c r="W40" s="57"/>
+      <c r="X40" s="57"/>
+      <c r="Y40" s="57"/>
+      <c r="Z40" s="44"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="43"/>
       <c r="B41" s="57"/>
       <c r="C41" s="57"/>
@@ -3150,9 +3452,17 @@
       <c r="O41" s="57"/>
       <c r="P41" s="57"/>
       <c r="Q41" s="57"/>
-      <c r="R41" s="44"/>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R41" s="57"/>
+      <c r="S41" s="57"/>
+      <c r="T41" s="57"/>
+      <c r="U41" s="57"/>
+      <c r="V41" s="57"/>
+      <c r="W41" s="57"/>
+      <c r="X41" s="57"/>
+      <c r="Y41" s="57"/>
+      <c r="Z41" s="44"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="45"/>
       <c r="B42" s="58"/>
       <c r="C42" s="58"/>
@@ -3170,9 +3480,17 @@
       <c r="O42" s="58"/>
       <c r="P42" s="58"/>
       <c r="Q42" s="58"/>
-      <c r="R42" s="46"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R42" s="58"/>
+      <c r="S42" s="58"/>
+      <c r="T42" s="58"/>
+      <c r="U42" s="58"/>
+      <c r="V42" s="58"/>
+      <c r="W42" s="58"/>
+      <c r="X42" s="58"/>
+      <c r="Y42" s="58"/>
+      <c r="Z42" s="46"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="24"/>
       <c r="B43" s="24"/>
       <c r="C43" s="24"/>
@@ -3192,7 +3510,7 @@
       <c r="Q43" s="24"/>
       <c r="R43" s="24"/>
     </row>
-    <row r="44" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:26" ht="21" x14ac:dyDescent="0.35">
       <c r="A44" s="29" t="s">
         <v>144</v>
       </c>
@@ -3214,7 +3532,7 @@
       <c r="Q44" s="24"/>
       <c r="R44" s="24"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="41"/>
       <c r="B45" s="56"/>
       <c r="C45" s="56"/>
@@ -3232,9 +3550,17 @@
       <c r="O45" s="56"/>
       <c r="P45" s="56"/>
       <c r="Q45" s="56"/>
-      <c r="R45" s="42"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R45" s="56"/>
+      <c r="S45" s="56"/>
+      <c r="T45" s="56"/>
+      <c r="U45" s="56"/>
+      <c r="V45" s="56"/>
+      <c r="W45" s="56"/>
+      <c r="X45" s="56"/>
+      <c r="Y45" s="56"/>
+      <c r="Z45" s="42"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="43"/>
       <c r="B46" s="57"/>
       <c r="C46" s="57"/>
@@ -3252,9 +3578,17 @@
       <c r="O46" s="57"/>
       <c r="P46" s="57"/>
       <c r="Q46" s="57"/>
-      <c r="R46" s="44"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R46" s="57"/>
+      <c r="S46" s="57"/>
+      <c r="T46" s="57"/>
+      <c r="U46" s="57"/>
+      <c r="V46" s="57"/>
+      <c r="W46" s="57"/>
+      <c r="X46" s="57"/>
+      <c r="Y46" s="57"/>
+      <c r="Z46" s="44"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="43"/>
       <c r="B47" s="57"/>
       <c r="C47" s="57"/>
@@ -3272,9 +3606,17 @@
       <c r="O47" s="57"/>
       <c r="P47" s="57"/>
       <c r="Q47" s="57"/>
-      <c r="R47" s="44"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R47" s="57"/>
+      <c r="S47" s="57"/>
+      <c r="T47" s="57"/>
+      <c r="U47" s="57"/>
+      <c r="V47" s="57"/>
+      <c r="W47" s="57"/>
+      <c r="X47" s="57"/>
+      <c r="Y47" s="57"/>
+      <c r="Z47" s="44"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="43"/>
       <c r="B48" s="57"/>
       <c r="C48" s="57"/>
@@ -3292,9 +3634,17 @@
       <c r="O48" s="57"/>
       <c r="P48" s="57"/>
       <c r="Q48" s="57"/>
-      <c r="R48" s="44"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R48" s="57"/>
+      <c r="S48" s="57"/>
+      <c r="T48" s="57"/>
+      <c r="U48" s="57"/>
+      <c r="V48" s="57"/>
+      <c r="W48" s="57"/>
+      <c r="X48" s="57"/>
+      <c r="Y48" s="57"/>
+      <c r="Z48" s="44"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="43"/>
       <c r="B49" s="57"/>
       <c r="C49" s="57"/>
@@ -3312,9 +3662,17 @@
       <c r="O49" s="57"/>
       <c r="P49" s="57"/>
       <c r="Q49" s="57"/>
-      <c r="R49" s="44"/>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R49" s="57"/>
+      <c r="S49" s="57"/>
+      <c r="T49" s="57"/>
+      <c r="U49" s="57"/>
+      <c r="V49" s="57"/>
+      <c r="W49" s="57"/>
+      <c r="X49" s="57"/>
+      <c r="Y49" s="57"/>
+      <c r="Z49" s="44"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="43"/>
       <c r="B50" s="57"/>
       <c r="C50" s="57"/>
@@ -3332,9 +3690,17 @@
       <c r="O50" s="57"/>
       <c r="P50" s="57"/>
       <c r="Q50" s="57"/>
-      <c r="R50" s="44"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R50" s="57"/>
+      <c r="S50" s="57"/>
+      <c r="T50" s="57"/>
+      <c r="U50" s="57"/>
+      <c r="V50" s="57"/>
+      <c r="W50" s="57"/>
+      <c r="X50" s="57"/>
+      <c r="Y50" s="57"/>
+      <c r="Z50" s="44"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="43"/>
       <c r="B51" s="57"/>
       <c r="C51" s="57"/>
@@ -3352,9 +3718,17 @@
       <c r="O51" s="57"/>
       <c r="P51" s="57"/>
       <c r="Q51" s="57"/>
-      <c r="R51" s="44"/>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R51" s="57"/>
+      <c r="S51" s="57"/>
+      <c r="T51" s="57"/>
+      <c r="U51" s="57"/>
+      <c r="V51" s="57"/>
+      <c r="W51" s="57"/>
+      <c r="X51" s="57"/>
+      <c r="Y51" s="57"/>
+      <c r="Z51" s="44"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="43"/>
       <c r="B52" s="57"/>
       <c r="C52" s="57"/>
@@ -3372,9 +3746,17 @@
       <c r="O52" s="57"/>
       <c r="P52" s="57"/>
       <c r="Q52" s="57"/>
-      <c r="R52" s="44"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R52" s="57"/>
+      <c r="S52" s="57"/>
+      <c r="T52" s="57"/>
+      <c r="U52" s="57"/>
+      <c r="V52" s="57"/>
+      <c r="W52" s="57"/>
+      <c r="X52" s="57"/>
+      <c r="Y52" s="57"/>
+      <c r="Z52" s="44"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="43"/>
       <c r="B53" s="57"/>
       <c r="C53" s="57"/>
@@ -3392,9 +3774,17 @@
       <c r="O53" s="57"/>
       <c r="P53" s="57"/>
       <c r="Q53" s="57"/>
-      <c r="R53" s="44"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R53" s="57"/>
+      <c r="S53" s="57"/>
+      <c r="T53" s="57"/>
+      <c r="U53" s="57"/>
+      <c r="V53" s="57"/>
+      <c r="W53" s="57"/>
+      <c r="X53" s="57"/>
+      <c r="Y53" s="57"/>
+      <c r="Z53" s="44"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="45"/>
       <c r="B54" s="58"/>
       <c r="C54" s="58"/>
@@ -3412,13 +3802,21 @@
       <c r="O54" s="58"/>
       <c r="P54" s="58"/>
       <c r="Q54" s="58"/>
-      <c r="R54" s="46"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R54" s="58"/>
+      <c r="S54" s="58"/>
+      <c r="T54" s="58"/>
+      <c r="U54" s="58"/>
+      <c r="V54" s="58"/>
+      <c r="W54" s="58"/>
+      <c r="X54" s="58"/>
+      <c r="Y54" s="58"/>
+      <c r="Z54" s="46"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H55" s="8"/>
       <c r="I55" s="5"/>
     </row>
-    <row r="56" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:26" ht="21" x14ac:dyDescent="0.35">
       <c r="A56" s="29" t="s">
         <v>145</v>
       </c>
@@ -3440,7 +3838,7 @@
       <c r="Q56" s="24"/>
       <c r="R56" s="24"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="41"/>
       <c r="B57" s="56"/>
       <c r="C57" s="56"/>
@@ -3458,9 +3856,17 @@
       <c r="O57" s="56"/>
       <c r="P57" s="56"/>
       <c r="Q57" s="56"/>
-      <c r="R57" s="42"/>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R57" s="56"/>
+      <c r="S57" s="56"/>
+      <c r="T57" s="56"/>
+      <c r="U57" s="56"/>
+      <c r="V57" s="56"/>
+      <c r="W57" s="56"/>
+      <c r="X57" s="56"/>
+      <c r="Y57" s="56"/>
+      <c r="Z57" s="42"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="43"/>
       <c r="B58" s="57"/>
       <c r="C58" s="57"/>
@@ -3478,9 +3884,17 @@
       <c r="O58" s="57"/>
       <c r="P58" s="57"/>
       <c r="Q58" s="57"/>
-      <c r="R58" s="44"/>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R58" s="57"/>
+      <c r="S58" s="57"/>
+      <c r="T58" s="57"/>
+      <c r="U58" s="57"/>
+      <c r="V58" s="57"/>
+      <c r="W58" s="57"/>
+      <c r="X58" s="57"/>
+      <c r="Y58" s="57"/>
+      <c r="Z58" s="44"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="43"/>
       <c r="B59" s="57"/>
       <c r="C59" s="57"/>
@@ -3498,9 +3912,17 @@
       <c r="O59" s="57"/>
       <c r="P59" s="57"/>
       <c r="Q59" s="57"/>
-      <c r="R59" s="44"/>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R59" s="57"/>
+      <c r="S59" s="57"/>
+      <c r="T59" s="57"/>
+      <c r="U59" s="57"/>
+      <c r="V59" s="57"/>
+      <c r="W59" s="57"/>
+      <c r="X59" s="57"/>
+      <c r="Y59" s="57"/>
+      <c r="Z59" s="44"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="43"/>
       <c r="B60" s="57"/>
       <c r="C60" s="57"/>
@@ -3518,9 +3940,17 @@
       <c r="O60" s="57"/>
       <c r="P60" s="57"/>
       <c r="Q60" s="57"/>
-      <c r="R60" s="44"/>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R60" s="57"/>
+      <c r="S60" s="57"/>
+      <c r="T60" s="57"/>
+      <c r="U60" s="57"/>
+      <c r="V60" s="57"/>
+      <c r="W60" s="57"/>
+      <c r="X60" s="57"/>
+      <c r="Y60" s="57"/>
+      <c r="Z60" s="44"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="43"/>
       <c r="B61" s="57"/>
       <c r="C61" s="57"/>
@@ -3538,9 +3968,17 @@
       <c r="O61" s="57"/>
       <c r="P61" s="57"/>
       <c r="Q61" s="57"/>
-      <c r="R61" s="44"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R61" s="57"/>
+      <c r="S61" s="57"/>
+      <c r="T61" s="57"/>
+      <c r="U61" s="57"/>
+      <c r="V61" s="57"/>
+      <c r="W61" s="57"/>
+      <c r="X61" s="57"/>
+      <c r="Y61" s="57"/>
+      <c r="Z61" s="44"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="43"/>
       <c r="B62" s="57"/>
       <c r="C62" s="57"/>
@@ -3558,9 +3996,17 @@
       <c r="O62" s="57"/>
       <c r="P62" s="57"/>
       <c r="Q62" s="57"/>
-      <c r="R62" s="44"/>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R62" s="57"/>
+      <c r="S62" s="57"/>
+      <c r="T62" s="57"/>
+      <c r="U62" s="57"/>
+      <c r="V62" s="57"/>
+      <c r="W62" s="57"/>
+      <c r="X62" s="57"/>
+      <c r="Y62" s="57"/>
+      <c r="Z62" s="44"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="43"/>
       <c r="B63" s="57"/>
       <c r="C63" s="57"/>
@@ -3578,9 +4024,17 @@
       <c r="O63" s="57"/>
       <c r="P63" s="57"/>
       <c r="Q63" s="57"/>
-      <c r="R63" s="44"/>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R63" s="57"/>
+      <c r="S63" s="57"/>
+      <c r="T63" s="57"/>
+      <c r="U63" s="57"/>
+      <c r="V63" s="57"/>
+      <c r="W63" s="57"/>
+      <c r="X63" s="57"/>
+      <c r="Y63" s="57"/>
+      <c r="Z63" s="44"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="43"/>
       <c r="B64" s="57"/>
       <c r="C64" s="57"/>
@@ -3598,9 +4052,17 @@
       <c r="O64" s="57"/>
       <c r="P64" s="57"/>
       <c r="Q64" s="57"/>
-      <c r="R64" s="44"/>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R64" s="57"/>
+      <c r="S64" s="57"/>
+      <c r="T64" s="57"/>
+      <c r="U64" s="57"/>
+      <c r="V64" s="57"/>
+      <c r="W64" s="57"/>
+      <c r="X64" s="57"/>
+      <c r="Y64" s="57"/>
+      <c r="Z64" s="44"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="43"/>
       <c r="B65" s="57"/>
       <c r="C65" s="57"/>
@@ -3618,9 +4080,17 @@
       <c r="O65" s="57"/>
       <c r="P65" s="57"/>
       <c r="Q65" s="57"/>
-      <c r="R65" s="44"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R65" s="57"/>
+      <c r="S65" s="57"/>
+      <c r="T65" s="57"/>
+      <c r="U65" s="57"/>
+      <c r="V65" s="57"/>
+      <c r="W65" s="57"/>
+      <c r="X65" s="57"/>
+      <c r="Y65" s="57"/>
+      <c r="Z65" s="44"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="45"/>
       <c r="B66" s="58"/>
       <c r="C66" s="58"/>
@@ -3638,32 +4108,40 @@
       <c r="O66" s="58"/>
       <c r="P66" s="58"/>
       <c r="Q66" s="58"/>
-      <c r="R66" s="46"/>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R66" s="58"/>
+      <c r="S66" s="58"/>
+      <c r="T66" s="58"/>
+      <c r="U66" s="58"/>
+      <c r="V66" s="58"/>
+      <c r="W66" s="58"/>
+      <c r="X66" s="58"/>
+      <c r="Y66" s="58"/>
+      <c r="Z66" s="46"/>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H67" s="8"/>
       <c r="I67" s="5"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H68" s="8"/>
       <c r="I68" s="5"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H69" s="8"/>
       <c r="I69" s="5"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H70" s="8"/>
       <c r="I70" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A2:R20"/>
-    <mergeCell ref="A23:R42"/>
-    <mergeCell ref="A45:R54"/>
-    <mergeCell ref="A57:R66"/>
+    <mergeCell ref="A2:Z20"/>
+    <mergeCell ref="A23:Z42"/>
+    <mergeCell ref="A45:Z54"/>
+    <mergeCell ref="A57:Z66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="51" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed broken Exit Strat label
</commit_message>
<xml_diff>
--- a/Src/SummitReports.Objects/Reports/UWRelationshipCashFlowReport/UW-RCF-Reports.xlsx
+++ b/Src/SummitReports.Objects/Reports/UWRelationshipCashFlowReport/UW-RCF-Reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Summit\SummitReports\Src\SummitReports.Objects\Reports\UWRelationshipCashFlowReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D4B179-1727-40EF-823D-1CC97406D9F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D6D918-4621-4031-A89E-FF60FB5A5490}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BidPoolData" sheetId="8" state="hidden" r:id="rId1"/>
@@ -1890,7 +1890,9 @@
   </sheetPr>
   <dimension ref="A2:S17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2170,10 +2172,11 @@
       <c r="D10" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="6" t="str">
+      <c r="E10" s="38" t="str">
         <f>RelationshipData!S1</f>
         <v>Bankruptcy</v>
       </c>
+      <c r="F10" s="39"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2347,7 +2350,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="C16:H16"/>
     <mergeCell ref="J16:S16"/>
     <mergeCell ref="G13:H13"/>
@@ -2359,6 +2362,7 @@
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="E11:F14"/>
     <mergeCell ref="B8:F8"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Added the ability to merge the rel xls files to one UW Relationship Master Report
</commit_message>
<xml_diff>
--- a/Src/SummitReports.Objects/Reports/UWRelationshipCashFlowReport/UW-RCF-Reports.xlsx
+++ b/Src/SummitReports.Objects/Reports/UWRelationshipCashFlowReport/UW-RCF-Reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Summit\SummitReports\Src\SummitReports.Objects\Reports\UWRelationshipCashFlowReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4C76A4-1869-413C-A914-48408365400A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AB45C3-3F4A-4C39-860C-4B87636CCE34}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5130" yWindow="17880" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MODEL" sheetId="10" r:id="rId1"/>
@@ -814,9 +814,7 @@
   </sheetPr>
   <dimension ref="A2:S17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -833,25 +831,16 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="14"/>
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="5" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="G2" s="5"/>
       <c r="I2" s="2" t="s">
         <v>25</v>
       </c>
@@ -875,52 +864,25 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B3" s="33"/>
       <c r="C3" s="34"/>
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="1" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="G3" s="1"/>
       <c r="H3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="17" t="e">
-        <f>I6+I9</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K3" s="18" t="e">
-        <f>K6+I9</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M3" s="11" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N3" s="13" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O3" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P3" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="I3" s="17"/>
+      <c r="K3" s="18"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H4"/>
@@ -930,18 +892,12 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="33" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B5" s="33"/>
       <c r="C5" s="34"/>
       <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="1" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="G5" s="1"/>
       <c r="I5" s="2" t="s">
         <v>26</v>
       </c>
@@ -968,78 +924,39 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="26" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B6" s="26"/>
       <c r="C6" s="19"/>
       <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="25" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="G6" s="25"/>
       <c r="H6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J6" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K6" s="18" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M6" s="10" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N6" s="10" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O6" s="9" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P6" s="9" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="18"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="33" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B7" s="33"/>
       <c r="C7" s="34"/>
-      <c r="D7" s="33" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D7" s="33"/>
       <c r="E7" s="34"/>
-      <c r="F7" s="1" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="F7" s="1"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="35" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B8" s="35"/>
       <c r="C8" s="43"/>
       <c r="D8" s="43"/>
       <c r="E8" s="43"/>
@@ -1063,61 +980,34 @@
       <c r="H9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="2" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M9" s="10" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N9" s="13" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O9" s="13" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P9" s="10" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="I9" s="2"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="10"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B10" s="4"/>
       <c r="C10" s="14"/>
       <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="35" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="E10" s="35"/>
       <c r="F10" s="36"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="35" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B11" s="35"/>
       <c r="C11" s="36"/>
       <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="37" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="E11" s="37"/>
       <c r="F11" s="38"/>
       <c r="M11" s="9" t="s">
         <v>39</v>
@@ -1136,38 +1026,20 @@
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="35" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B12" s="35"/>
       <c r="C12" s="36"/>
       <c r="E12" s="39"/>
       <c r="F12" s="40"/>
-      <c r="M12" s="11" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N12" s="11" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O12" s="11" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P12" s="11" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="21" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B13" s="21"/>
       <c r="C13" s="20"/>
       <c r="E13" s="39"/>
       <c r="F13" s="40"/>
@@ -1175,22 +1047,10 @@
         <v>24</v>
       </c>
       <c r="H13" s="32"/>
-      <c r="I13" s="2" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J13" s="2" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K13" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L13" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E14" s="41"/>

</xml_diff>